<commit_message>
configure CHT outbound for the emr
</commit_message>
<xml_diff>
--- a/config/default/forms/app/hts_linkage.xlsx
+++ b/config/default/forms/app/hts_linkage.xlsx
@@ -1,19 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Test\Desktop\kpif\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B572481-F12A-4F9A-9F5C-AAADF06BD352}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView minimized="1" xWindow="7590" yWindow="2220" windowWidth="4500" windowHeight="2355" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="choices" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="settings" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="survey" sheetId="1" r:id="rId1"/>
+    <sheet name="choices" sheetId="2" r:id="rId2"/>
+    <sheet name="settings" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
@@ -22,399 +35,376 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="101">
-  <si>
-    <t xml:space="preserve">type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">label</t>
-  </si>
-  <si>
-    <t xml:space="preserve">required</t>
-  </si>
-  <si>
-    <t xml:space="preserve">relevant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">appearance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">constraint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">constraint_message::en</t>
-  </si>
-  <si>
-    <t xml:space="preserve">calculation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">choice_filter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">default</t>
-  </si>
-  <si>
-    <t xml:space="preserve">media::image</t>
-  </si>
-  <si>
-    <t xml:space="preserve">begin group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inputs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Patient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./source = 'user'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">field-list</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hidden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">source</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Source</t>
-  </si>
-  <si>
-    <t xml:space="preserve">user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">source_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Source ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contact</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact</t>
-  </si>
-  <si>
-    <t xml:space="preserve">db:clinic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What is the patient's name?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">db-object</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">db:person</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID of head of household</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name of head of household</t>
-  </si>
-  <si>
-    <t xml:space="preserve">end group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">parent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHW name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHW phone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">calculate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NO_LABEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../inputs/source</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../inputs/source_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">place_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../inputs/contact/_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">place_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../inputs/contact/name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">head</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../inputs/contact/contact/name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hts_linkage_assessment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Linkage to care</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">encounter_date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Encounter Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">facility_linkedto_name</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="102">
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>relevant</t>
+  </si>
+  <si>
+    <t>appearance</t>
+  </si>
+  <si>
+    <t>constraint</t>
+  </si>
+  <si>
+    <t>constraint_message::en</t>
+  </si>
+  <si>
+    <t>calculation</t>
+  </si>
+  <si>
+    <t>choice_filter</t>
+  </si>
+  <si>
+    <t>hint</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>media::image</t>
+  </si>
+  <si>
+    <t>begin group</t>
+  </si>
+  <si>
+    <t>inputs</t>
+  </si>
+  <si>
+    <t>Patient</t>
+  </si>
+  <si>
+    <t>./source = 'user'</t>
+  </si>
+  <si>
+    <t>field-list</t>
+  </si>
+  <si>
+    <t>hidden</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>source_id</t>
+  </si>
+  <si>
+    <t>Source ID</t>
+  </si>
+  <si>
+    <t>contact</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>db:clinic</t>
+  </si>
+  <si>
+    <t>_id</t>
+  </si>
+  <si>
+    <t>What is the patient's name?</t>
+  </si>
+  <si>
+    <t>db-object</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>db:person</t>
+  </si>
+  <si>
+    <t>ID of head of household</t>
+  </si>
+  <si>
+    <t>Name of head of household</t>
+  </si>
+  <si>
+    <t>end group</t>
+  </si>
+  <si>
+    <t>parent</t>
+  </si>
+  <si>
+    <t>Parent</t>
+  </si>
+  <si>
+    <t>CHW name</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>CHW phone</t>
+  </si>
+  <si>
+    <t>calculate</t>
+  </si>
+  <si>
+    <t>NO_LABEL</t>
+  </si>
+  <si>
+    <t>../inputs/source</t>
+  </si>
+  <si>
+    <t>../inputs/source_id</t>
+  </si>
+  <si>
+    <t>place_id</t>
+  </si>
+  <si>
+    <t>../inputs/contact/_id</t>
+  </si>
+  <si>
+    <t>place_name</t>
+  </si>
+  <si>
+    <t>../inputs/contact/name</t>
+  </si>
+  <si>
+    <t>head</t>
+  </si>
+  <si>
+    <t>../inputs/contact/contact/name</t>
+  </si>
+  <si>
+    <t>hts_linkage_assessment</t>
+  </si>
+  <si>
+    <t>Linkage to care</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Encounter Date</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>text</t>
   </si>
   <si>
     <t xml:space="preserve">Facility linked to:  </t>
   </si>
   <si>
-    <t xml:space="preserve"> ccc_number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCC number:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">health_worker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Health worker handed to</t>
-  </si>
-  <si>
-    <t xml:space="preserve">select_one cadre_of_health_worker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cadre_worker</t>
+    <t>CCC number:</t>
+  </si>
+  <si>
+    <t>Health worker handed to</t>
+  </si>
+  <si>
+    <t>select_one cadre_of_health_worker</t>
   </si>
   <si>
     <t xml:space="preserve">Cadre of health worker : </t>
   </si>
   <si>
-    <t xml:space="preserve">other_cadre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Specify other cadre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${cadre_worker}=”other”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date_enrolled</t>
+    <t>Specify other cadre</t>
   </si>
   <si>
     <t xml:space="preserve">Date enrolled : </t>
   </si>
   <si>
-    <t xml:space="preserve">Art-date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ART start date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">remark</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Remark(s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">list_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes_no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cadre_of_health_worker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nurse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nurse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">clinical_officer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clincal officer/Docter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">community_health</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Community health care worker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">employee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Employee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">other</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other</t>
-  </si>
-  <si>
-    <t xml:space="preserve">form_title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">form_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">version</t>
-  </si>
-  <si>
-    <t xml:space="preserve">style</t>
-  </si>
-  <si>
-    <t xml:space="preserve">path</t>
-  </si>
-  <si>
-    <t xml:space="preserve">instance_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HTS Linkage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hts_linkage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pages</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data</t>
+    <t>ART start date</t>
+  </si>
+  <si>
+    <t>Remark(s)</t>
+  </si>
+  <si>
+    <t>list_name</t>
+  </si>
+  <si>
+    <t>yes_no</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>cadre_of_health_worker</t>
+  </si>
+  <si>
+    <t>Nurse</t>
+  </si>
+  <si>
+    <t>Clincal officer/Docter</t>
+  </si>
+  <si>
+    <t>Community health care worker</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>form_title</t>
+  </si>
+  <si>
+    <t>form_id</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>style</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>instance_name</t>
+  </si>
+  <si>
+    <t>HTS Linkage</t>
+  </si>
+  <si>
+    <t>hts_linkage</t>
+  </si>
+  <si>
+    <t>pages</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>_164401_otherCadre_99DCT</t>
+  </si>
+  <si>
+    <t>_162724_facilityLinkedTo_99DCT</t>
+  </si>
+  <si>
+    <t>_162053_cccNumber_99DCT</t>
+  </si>
+  <si>
+    <t>_1473_healthWorkerHandedTo_99DCT</t>
+  </si>
+  <si>
+    <t>_162577_cadreOfHealthWorker_99DCT</t>
+  </si>
+  <si>
+    <t>_160555_dateEnrolled_99DCT</t>
+  </si>
+  <si>
+    <t>_159599_ARTdate_99DCT</t>
+  </si>
+  <si>
+    <t>_163042_remarks_99DCT</t>
+  </si>
+  <si>
+    <t>_1577_nurse_99DCT</t>
+  </si>
+  <si>
+    <t>_1574_clinicalOficer_99DCT</t>
+  </si>
+  <si>
+    <t>_1555_communityHealthWorker_99DCT</t>
+  </si>
+  <si>
+    <t>_1540_employess_99DCT</t>
+  </si>
+  <si>
+    <t>_5622_other_99DCT</t>
+  </si>
+  <si>
+    <t>_1065_yes_99DCT</t>
+  </si>
+  <si>
+    <t>_1066_no_99DCT</t>
+  </si>
+  <si>
+    <t>_163137_encounterDAte_99DCT</t>
+  </si>
+  <si>
+    <t>${_162577_cadreOfHealthWorker_99DCT}=”_5622_other_99DCT”</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD\-MM\-YYYY\ HH\-MM\-SS"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy\ hh\-mm\-ss"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFA9B7C6"/>
       <name val="DejaVu Sans Mono"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF4C4C4C"/>
       <name val="Ubuntu"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFCCCCCC"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Cambria"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Cambria"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="4">
@@ -438,7 +428,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -446,117 +436,69 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="26">
     <dxf>
       <font>
-        <color rgb="FFB7B7B7"/>
+        <color rgb="FFC27BA0"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9D2E9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -566,55 +508,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFCFE2F3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC27BA0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCFE2F3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFCCCCCC"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFCE5CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="1"/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF980000"/>
+          <bgColor rgb="FFD9D2E9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -626,9 +520,141 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFFFFFF"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEAD1DC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -645,7 +671,62 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFEAD1DC"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF980000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCCCCCC"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC27BA0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCFE2F3"/>
         </patternFill>
       </fill>
     </dxf>
@@ -655,21 +736,22 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFD9D2E9"/>
+          <bgColor rgb="FFCFE2F3"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFC27BA0"/>
+        <color rgb="FFB7B7B7"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFD9D2E9"/>
+          <bgColor rgb="FFD9EAD3"/>
         </patternFill>
       </fill>
     </dxf>
   </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -728,45 +810,352 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF4C4C4C"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B34" activeCellId="0" sqref="B34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C27" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="48.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="52.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="38.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="32.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="73.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="25.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="13" style="0" width="29.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="26" style="0" width="14.43"/>
+    <col min="1" max="1" width="28.1328125" customWidth="1"/>
+    <col min="2" max="2" width="28.265625" customWidth="1"/>
+    <col min="3" max="3" width="48.53125" customWidth="1"/>
+    <col min="4" max="4" width="14.3984375" customWidth="1"/>
+    <col min="5" max="5" width="52.3984375" customWidth="1"/>
+    <col min="6" max="6" width="17.3984375" customWidth="1"/>
+    <col min="7" max="7" width="38.6640625" customWidth="1"/>
+    <col min="8" max="8" width="32.73046875" customWidth="1"/>
+    <col min="9" max="9" width="73.86328125" customWidth="1"/>
+    <col min="10" max="10" width="14.3984375" customWidth="1"/>
+    <col min="11" max="11" width="25.1328125" customWidth="1"/>
+    <col min="12" max="12" width="14.3984375" customWidth="1"/>
+    <col min="13" max="25" width="29.86328125" customWidth="1"/>
+    <col min="26" max="1025" width="14.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:25" ht="13.9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -819,7 +1208,7 @@
       <c r="X1" s="2"/>
       <c r="Y1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:25" ht="13.5">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -856,7 +1245,7 @@
       <c r="X2" s="4"/>
       <c r="Y2" s="4"/>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:25" ht="13.5">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -891,7 +1280,7 @@
       <c r="X3" s="4"/>
       <c r="Y3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:25" ht="13.5">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
@@ -924,7 +1313,7 @@
       <c r="X4" s="4"/>
       <c r="Y4" s="4"/>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:25" ht="13.5">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -957,7 +1346,7 @@
       <c r="X5" s="4"/>
       <c r="Y5" s="4"/>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:25" ht="13.5">
       <c r="A6" s="3" t="s">
         <v>26</v>
       </c>
@@ -992,7 +1381,7 @@
       <c r="X6" s="4"/>
       <c r="Y6" s="4"/>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:25" ht="13.5">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -1025,7 +1414,7 @@
       <c r="X7" s="4"/>
       <c r="Y7" s="4"/>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:25" ht="13.5">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
@@ -1058,7 +1447,7 @@
       <c r="X8" s="4"/>
       <c r="Y8" s="4"/>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:25" ht="13.5">
       <c r="A9" s="3" t="s">
         <v>31</v>
       </c>
@@ -1093,7 +1482,7 @@
       <c r="X9" s="4"/>
       <c r="Y9" s="4"/>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:25" ht="13.5">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
@@ -1126,7 +1515,7 @@
       <c r="X10" s="4"/>
       <c r="Y10" s="4"/>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:25" ht="13.5">
       <c r="A11" s="3" t="s">
         <v>34</v>
       </c>
@@ -1155,7 +1544,7 @@
       <c r="X11" s="4"/>
       <c r="Y11" s="4"/>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:25" ht="13.5">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
@@ -1188,7 +1577,7 @@
       <c r="X12" s="4"/>
       <c r="Y12" s="4"/>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:25" ht="13.5">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
@@ -1221,7 +1610,7 @@
       <c r="X13" s="4"/>
       <c r="Y13" s="4"/>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:25" ht="13.5">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -1254,7 +1643,7 @@
       <c r="X14" s="4"/>
       <c r="Y14" s="4"/>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:25" ht="13.5">
       <c r="A15" s="3" t="s">
         <v>18</v>
       </c>
@@ -1287,7 +1676,7 @@
       <c r="X15" s="4"/>
       <c r="Y15" s="4"/>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:25" ht="13.5">
       <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
@@ -1320,7 +1709,7 @@
       <c r="X16" s="4"/>
       <c r="Y16" s="4"/>
     </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:25" ht="13.5">
       <c r="A17" s="3" t="s">
         <v>34</v>
       </c>
@@ -1349,7 +1738,7 @@
       <c r="X17" s="4"/>
       <c r="Y17" s="4"/>
     </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:25" ht="13.5">
       <c r="A18" s="3" t="s">
         <v>34</v>
       </c>
@@ -1378,7 +1767,7 @@
       <c r="X18" s="4"/>
       <c r="Y18" s="4"/>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:25" ht="13.5">
       <c r="A19" s="3" t="s">
         <v>34</v>
       </c>
@@ -1407,7 +1796,7 @@
       <c r="X19" s="4"/>
       <c r="Y19" s="4"/>
     </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:25" ht="13.5">
       <c r="A20" s="3" t="s">
         <v>34</v>
       </c>
@@ -1436,7 +1825,7 @@
       <c r="X20" s="4"/>
       <c r="Y20" s="4"/>
     </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:25" ht="13.5">
       <c r="A21" s="3" t="s">
         <v>34</v>
       </c>
@@ -1465,7 +1854,7 @@
       <c r="X21" s="4"/>
       <c r="Y21" s="4"/>
     </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:25" ht="13.5">
       <c r="A22" s="3" t="s">
         <v>40</v>
       </c>
@@ -1500,7 +1889,7 @@
       <c r="X22" s="4"/>
       <c r="Y22" s="4"/>
     </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:25" ht="13.5">
       <c r="A23" s="3" t="s">
         <v>40</v>
       </c>
@@ -1535,7 +1924,7 @@
       <c r="X23" s="4"/>
       <c r="Y23" s="4"/>
     </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:25" ht="13.5">
       <c r="A24" s="5" t="s">
         <v>40</v>
       </c>
@@ -1570,7 +1959,7 @@
       <c r="X24" s="5"/>
       <c r="Y24" s="5"/>
     </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:25" ht="13.5">
       <c r="A25" s="5" t="s">
         <v>40</v>
       </c>
@@ -1605,7 +1994,7 @@
       <c r="X25" s="5"/>
       <c r="Y25" s="5"/>
     </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:25" ht="13.5">
       <c r="A26" s="5" t="s">
         <v>40</v>
       </c>
@@ -1640,7 +2029,7 @@
       <c r="X26" s="5"/>
       <c r="Y26" s="5"/>
     </row>
-    <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:25" ht="13.5">
       <c r="A27" s="5" t="s">
         <v>13</v>
       </c>
@@ -1675,18 +2064,18 @@
       <c r="X27" s="5"/>
       <c r="Y27" s="5"/>
     </row>
-    <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:25" ht="13.5">
       <c r="A28" s="5" t="s">
         <v>52</v>
       </c>
       <c r="B28" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C28" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="D28" s="5" t="s">
         <v>54</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>55</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
@@ -1710,18 +2099,18 @@
       <c r="X28" s="5"/>
       <c r="Y28" s="5"/>
     </row>
-    <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:25" ht="27">
       <c r="A29" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>58</v>
-      </c>
       <c r="D29" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
@@ -1745,18 +2134,18 @@
       <c r="X29" s="5"/>
       <c r="Y29" s="5"/>
     </row>
-    <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:25" ht="13.5">
       <c r="A30" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>59</v>
+        <v>87</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
@@ -1780,18 +2169,18 @@
       <c r="X30" s="5"/>
       <c r="Y30" s="5"/>
     </row>
-    <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:25" ht="27">
       <c r="A31" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
@@ -1815,15 +2204,15 @@
       <c r="X31" s="5"/>
       <c r="Y31" s="5"/>
     </row>
-    <row r="32" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:25" ht="27">
       <c r="A32" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
@@ -1848,7 +2237,7 @@
       <c r="X32" s="5"/>
       <c r="Y32" s="5"/>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:25" ht="13.5">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -1875,19 +2264,19 @@
       <c r="X33" s="5"/>
       <c r="Y33" s="5"/>
     </row>
-    <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:25" ht="27">
       <c r="A34" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="8" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
@@ -1910,7 +2299,7 @@
       <c r="X34" s="5"/>
       <c r="Y34" s="5"/>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:25" ht="13.5">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -1937,18 +2326,18 @@
       <c r="X35" s="5"/>
       <c r="Y35" s="5"/>
     </row>
-    <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:25" ht="13.5">
       <c r="A36" s="5" t="s">
         <v>52</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>69</v>
+        <v>90</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
@@ -1972,18 +2361,18 @@
       <c r="X36" s="5"/>
       <c r="Y36" s="5"/>
     </row>
-    <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:25" ht="13.5">
       <c r="A37" s="5" t="s">
         <v>52</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
@@ -2007,15 +2396,15 @@
       <c r="X37" s="5"/>
       <c r="Y37" s="5"/>
     </row>
-    <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:25" ht="13.5">
       <c r="A38" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
@@ -2040,7 +2429,7 @@
       <c r="X38" s="5"/>
       <c r="Y38" s="5"/>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:25" ht="13.5">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -2067,7 +2456,7 @@
       <c r="X39" s="5"/>
       <c r="Y39" s="5"/>
     </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:25" ht="13.5">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -2094,7 +2483,7 @@
       <c r="X40" s="5"/>
       <c r="Y40" s="5"/>
     </row>
-    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:25" ht="13.5">
       <c r="A41" s="5" t="s">
         <v>34</v>
       </c>
@@ -2123,7 +2512,7 @@
       <c r="X41" s="5"/>
       <c r="Y41" s="5"/>
     </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:25" ht="13.5">
       <c r="A42" s="4"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
@@ -2150,7 +2539,7 @@
       <c r="X42" s="5"/>
       <c r="Y42" s="5"/>
     </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:25" ht="13.5">
       <c r="A43" s="4"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -2177,7 +2566,7 @@
       <c r="X43" s="5"/>
       <c r="Y43" s="5"/>
     </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:25" ht="13.5">
       <c r="A44" s="4"/>
       <c r="B44" s="5"/>
       <c r="C44" s="7"/>
@@ -2204,7 +2593,7 @@
       <c r="X44" s="5"/>
       <c r="Y44" s="5"/>
     </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:25" ht="13.5">
       <c r="A45" s="4"/>
       <c r="B45" s="5"/>
       <c r="C45" s="7"/>
@@ -2231,7 +2620,7 @@
       <c r="X45" s="5"/>
       <c r="Y45" s="5"/>
     </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:25" ht="13.5">
       <c r="A46" s="4"/>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
@@ -2258,7 +2647,7 @@
       <c r="X46" s="5"/>
       <c r="Y46" s="5"/>
     </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:25" ht="13.5">
       <c r="A47" s="4"/>
       <c r="B47" s="9"/>
       <c r="C47" s="4"/>
@@ -2285,7 +2674,7 @@
       <c r="X47" s="4"/>
       <c r="Y47" s="4"/>
     </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:25" ht="13.5">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -2312,7 +2701,7 @@
       <c r="X48" s="4"/>
       <c r="Y48" s="4"/>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" spans="1:25" ht="13.5">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
@@ -2339,7 +2728,7 @@
       <c r="X49" s="4"/>
       <c r="Y49" s="4"/>
     </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" spans="1:25" ht="13.5">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -2366,7 +2755,7 @@
       <c r="X50" s="4"/>
       <c r="Y50" s="4"/>
     </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:25" ht="13.5">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -2393,7 +2782,7 @@
       <c r="X51" s="4"/>
       <c r="Y51" s="4"/>
     </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" spans="1:25" ht="13.5">
       <c r="A52" s="5"/>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
@@ -2420,7 +2809,7 @@
       <c r="X52" s="5"/>
       <c r="Y52" s="5"/>
     </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" spans="1:25" ht="13.5">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="7"/>
@@ -2447,7 +2836,7 @@
       <c r="X53" s="4"/>
       <c r="Y53" s="4"/>
     </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:25" ht="13.5">
       <c r="A54" s="4"/>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
@@ -2474,7 +2863,7 @@
       <c r="X54" s="5"/>
       <c r="Y54" s="5"/>
     </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" spans="1:25" ht="13.5">
       <c r="A55" s="4"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
@@ -2501,7 +2890,7 @@
       <c r="X55" s="5"/>
       <c r="Y55" s="5"/>
     </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" spans="1:25" ht="13.5">
       <c r="A56" s="5"/>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
@@ -2528,7 +2917,7 @@
       <c r="X56" s="5"/>
       <c r="Y56" s="5"/>
     </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" spans="1:25" ht="13.5">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
@@ -2555,7 +2944,7 @@
       <c r="X57" s="4"/>
       <c r="Y57" s="4"/>
     </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" spans="1:25" ht="13.5">
       <c r="A58" s="4"/>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
@@ -2582,7 +2971,7 @@
       <c r="X58" s="5"/>
       <c r="Y58" s="5"/>
     </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" spans="1:25" ht="13.5">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
@@ -2609,7 +2998,7 @@
       <c r="X59" s="4"/>
       <c r="Y59" s="4"/>
     </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" spans="1:25" ht="13.5">
       <c r="A60" s="5"/>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
@@ -2636,7 +3025,7 @@
       <c r="X60" s="5"/>
       <c r="Y60" s="5"/>
     </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" spans="1:25" ht="13.5">
       <c r="A61" s="10"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
@@ -2663,7 +3052,7 @@
       <c r="X61" s="11"/>
       <c r="Y61" s="11"/>
     </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" spans="1:25" ht="13.5">
       <c r="A62" s="10"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
@@ -2690,7 +3079,7 @@
       <c r="X62" s="11"/>
       <c r="Y62" s="11"/>
     </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" spans="1:25" ht="13.5">
       <c r="A63" s="10"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
@@ -2717,188 +3106,161 @@
       <c r="X63" s="11"/>
       <c r="Y63" s="11"/>
     </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" ht="15.75" customHeight="1"/>
   </sheetData>
   <conditionalFormatting sqref="A1:Y1019">
-    <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
+    <cfRule type="containsText" dxfId="25" priority="2" operator="containsText" text="calculate"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Y1004">
-    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" dxfId="24" priority="3">
       <formula>AND($A1="begin group", NOT($B1 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Y1019">
-    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" dxfId="23" priority="4">
       <formula>AND($A1="end group", $B1 = "", $C1 = "", $D1 = "", $E1 = "", $F1 = "", $G1 = "", $H1 = "", $I1 = "", $J1 = "", $K1 = "", $L1 = "", $M1 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Y1019">
-    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" dxfId="22" priority="5" operator="equal">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+    <cfRule type="expression" dxfId="21" priority="6">
       <formula>AND(A1 = "type", COUNTIF($A$1:$A$1013, "begin group") = COUNTIF($A$1:$A$1013, "end group"))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="expression" dxfId="20" priority="7">
       <formula>OR(NOT(A1 = "type"), NOT(COUNTIF($A$1:$A$1004, "begin group") = COUNTIF($A$1:$A$1013, "end group")))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1019">
-    <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" dxfId="19" priority="8">
       <formula>AND($I1 = "", $A1 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1019">
-    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" dxfId="18" priority="9">
       <formula>AND(AND(NOT($A1 = "end group"), NOT($A1 = "end repeat"), NOT($A1 = "")), $C1 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1019">
-    <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="expression" dxfId="17" priority="10">
       <formula>AND(AND(NOT($A1 = "end group"), NOT($A1 = "end repeat"), NOT($A1 = "")), $B1 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1019">
-    <cfRule type="cellIs" priority="11" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" dxfId="16" priority="11" operator="equal">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B1012">
-    <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="expression" dxfId="15" priority="12">
       <formula>COUNTIF($B$2:$B$1012,B2)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1">
-    <cfRule type="cellIs" priority="13" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="notEqual">
       <formula>"name"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1">
-    <cfRule type="notContainsText" priority="14" operator="notContains" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="label" dxfId="5"/>
+    <cfRule type="notContainsText" dxfId="13" priority="14" operator="notContains" text="label"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1">
-    <cfRule type="cellIs" priority="15" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="cellIs" dxfId="12" priority="15" operator="notEqual">
       <formula>"required"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1">
-    <cfRule type="cellIs" priority="16" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="cellIs" dxfId="11" priority="16" operator="notEqual">
       <formula>"relevant"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="cellIs" priority="17" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="cellIs" dxfId="10" priority="17" operator="notEqual">
       <formula>"appearance"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1">
-    <cfRule type="cellIs" priority="18" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="cellIs" dxfId="9" priority="18" operator="notEqual">
       <formula>"constraint"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="notContainsText" priority="19" operator="notContains" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="constraint_message" dxfId="5"/>
+    <cfRule type="notContainsText" dxfId="8" priority="19" operator="notContains" text="constraint_message"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1">
-    <cfRule type="cellIs" priority="20" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="cellIs" dxfId="7" priority="20" operator="notEqual">
       <formula>"calculation"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1">
-    <cfRule type="cellIs" priority="21" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="cellIs" dxfId="6" priority="21" operator="notEqual">
       <formula>"choice_filter"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1">
-    <cfRule type="notContainsText" priority="22" operator="notContains" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="hint" dxfId="5"/>
+    <cfRule type="notContainsText" dxfId="5" priority="22" operator="notContains" text="hint"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1">
-    <cfRule type="cellIs" priority="23" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="cellIs" dxfId="4" priority="23" operator="notEqual">
       <formula>"default"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:Y1">
-    <cfRule type="cellIs" priority="24" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="cellIs" dxfId="3" priority="24" operator="notEqual">
       <formula>"media::image"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1004">
-    <cfRule type="expression" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" dxfId="2" priority="25">
       <formula>AND(NOT($G1 = ""), $H1 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Y1004">
-    <cfRule type="expression" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" dxfId="1" priority="26">
       <formula>AND($A1="begin repeat", NOT($B1 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Y1019">
-    <cfRule type="expression" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" dxfId="0" priority="27">
       <formula>AND($A1="end repeat", $B1 = "", $C1 = "", $D1 = "", $E1 = "", $F1 = "", $G1 = "", $H1 = "", $I1 = "", $J1 = "", $K1 = "", $L1 = "", $M1 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D2:D63" type="list">
+    <dataValidation type="list" allowBlank="1" sqref="D2:D63" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"yes,no"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="39.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="14.43"/>
+    <col min="1" max="1" width="25.53125" customWidth="1"/>
+    <col min="2" max="2" width="31.1328125" customWidth="1"/>
+    <col min="3" max="3" width="39.1328125" customWidth="1"/>
+    <col min="4" max="1025" width="14.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="13.9">
       <c r="A1" s="12" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>1</v>
@@ -2910,35 +3272,35 @@
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="13.5">
       <c r="A2" s="14" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>55</v>
+        <v>98</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="D2" s="14"/>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" ht="13.5">
       <c r="A3" s="14" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
       <c r="F3" s="14"/>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:6" ht="13.5">
       <c r="A4" s="14"/>
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
@@ -2946,167 +3308,141 @@
       <c r="E4" s="14"/>
       <c r="F4" s="14"/>
     </row>
-    <row r="5" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:6" ht="13.5">
       <c r="A5" s="14" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="14"/>
       <c r="F5" s="14"/>
     </row>
-    <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:6" ht="13.5">
       <c r="A6" s="14" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
     </row>
-    <row r="7" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:6" ht="27">
       <c r="A7" s="14" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
     </row>
-    <row r="8" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:6" ht="13.5">
       <c r="A8" s="15" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
     </row>
-    <row r="9" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:6" ht="13.5">
       <c r="A9" s="15" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="14.43"/>
+    <col min="1" max="2" width="14.3984375" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="4" max="1025" width="14.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="27.75">
       <c r="A1" s="12" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="13.5">
       <c r="A2" s="14" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="C2" s="16" t="n">
-        <f aca="true">NOW()</f>
-        <v>43962.8095109681</v>
+        <v>82</v>
+      </c>
+      <c r="C2" s="16">
+        <f ca="1">NOW()</f>
+        <v>44054.403139699076</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="F2" s="14"/>
     </row>
-    <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added outbound for contact listing
</commit_message>
<xml_diff>
--- a/config/default/forms/app/hts_linkage.xlsx
+++ b/config/default/forms/app/hts_linkage.xlsx
@@ -1,32 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Test\Desktop\kpif\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B572481-F12A-4F9A-9F5C-AAADF06BD352}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView minimized="1" xWindow="7590" yWindow="2220" windowWidth="4500" windowHeight="2355" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="996" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="survey" sheetId="1" r:id="rId1"/>
-    <sheet name="choices" sheetId="2" r:id="rId2"/>
-    <sheet name="settings" sheetId="3" r:id="rId3"/>
+    <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="choices" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="settings" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
@@ -35,376 +22,405 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="102">
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>label</t>
-  </si>
-  <si>
-    <t>required</t>
-  </si>
-  <si>
-    <t>relevant</t>
-  </si>
-  <si>
-    <t>appearance</t>
-  </si>
-  <si>
-    <t>constraint</t>
-  </si>
-  <si>
-    <t>constraint_message::en</t>
-  </si>
-  <si>
-    <t>calculation</t>
-  </si>
-  <si>
-    <t>choice_filter</t>
-  </si>
-  <si>
-    <t>hint</t>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
-    <t>media::image</t>
-  </si>
-  <si>
-    <t>begin group</t>
-  </si>
-  <si>
-    <t>inputs</t>
-  </si>
-  <si>
-    <t>Patient</t>
-  </si>
-  <si>
-    <t>./source = 'user'</t>
-  </si>
-  <si>
-    <t>field-list</t>
-  </si>
-  <si>
-    <t>hidden</t>
-  </si>
-  <si>
-    <t>source</t>
-  </si>
-  <si>
-    <t>Source</t>
-  </si>
-  <si>
-    <t>user</t>
-  </si>
-  <si>
-    <t>source_id</t>
-  </si>
-  <si>
-    <t>Source ID</t>
-  </si>
-  <si>
-    <t>contact</t>
-  </si>
-  <si>
-    <t>Contact</t>
-  </si>
-  <si>
-    <t>db:clinic</t>
-  </si>
-  <si>
-    <t>_id</t>
-  </si>
-  <si>
-    <t>What is the patient's name?</t>
-  </si>
-  <si>
-    <t>db-object</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>db:person</t>
-  </si>
-  <si>
-    <t>ID of head of household</t>
-  </si>
-  <si>
-    <t>Name of head of household</t>
-  </si>
-  <si>
-    <t>end group</t>
-  </si>
-  <si>
-    <t>parent</t>
-  </si>
-  <si>
-    <t>Parent</t>
-  </si>
-  <si>
-    <t>CHW name</t>
-  </si>
-  <si>
-    <t>phone</t>
-  </si>
-  <si>
-    <t>CHW phone</t>
-  </si>
-  <si>
-    <t>calculate</t>
-  </si>
-  <si>
-    <t>NO_LABEL</t>
-  </si>
-  <si>
-    <t>../inputs/source</t>
-  </si>
-  <si>
-    <t>../inputs/source_id</t>
-  </si>
-  <si>
-    <t>place_id</t>
-  </si>
-  <si>
-    <t>../inputs/contact/_id</t>
-  </si>
-  <si>
-    <t>place_name</t>
-  </si>
-  <si>
-    <t>../inputs/contact/name</t>
-  </si>
-  <si>
-    <t>head</t>
-  </si>
-  <si>
-    <t>../inputs/contact/contact/name</t>
-  </si>
-  <si>
-    <t>hts_linkage_assessment</t>
-  </si>
-  <si>
-    <t>Linkage to care</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>Encounter Date</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>text</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="104">
+  <si>
+    <t xml:space="preserve">type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">required</t>
+  </si>
+  <si>
+    <t xml:space="preserve">relevant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">appearance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">constraint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">constraint_message::en</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calculation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">choice_filter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">media::image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">begin group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inputs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./source = 'user'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">field-list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hidden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">source_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">db:clinic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is the patient's name?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">db-object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">db:person</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID of head of household</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name of head of household</t>
+  </si>
+  <si>
+    <t xml:space="preserve">end group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHW name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHW phone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calculate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO_LABEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../inputs/source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../inputs/source_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">place_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../inputs/contact/_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">place_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../inputs/contact/name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">head</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../inputs/contact/contact/name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">form_uuid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'050a7f12-5c52-4cad-8834-863695af335d'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">encounter_type_uuid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'9c0a7a57-62ff-4f75-babe-5835b0e921b7'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">observation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linkage to care</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_162724_facilityLinkedTo_99DCT</t>
   </si>
   <si>
     <t xml:space="preserve">Facility linked to:  </t>
   </si>
   <si>
-    <t>CCC number:</t>
-  </si>
-  <si>
-    <t>Health worker handed to</t>
-  </si>
-  <si>
-    <t>select_one cadre_of_health_worker</t>
+    <t xml:space="preserve">yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_162053_cccNumber_99DCT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCC number:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_1473_healthWorkerHandedTo_99DCT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Health worker handed to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one cadre_of_health_worker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_162577_cadreOfHealthWorker_99DCT</t>
   </si>
   <si>
     <t xml:space="preserve">Cadre of health worker : </t>
   </si>
   <si>
-    <t>Specify other cadre</t>
+    <t xml:space="preserve">_164401_otherCadre_99DCT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specify other cadre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${_162577_cadreOfHealthWorker_99DCT}=”_5622_other_99DCT”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_160555_dateEnrolled_99DCT</t>
   </si>
   <si>
     <t xml:space="preserve">Date enrolled : </t>
   </si>
   <si>
-    <t>ART start date</t>
-  </si>
-  <si>
-    <t>Remark(s)</t>
-  </si>
-  <si>
-    <t>list_name</t>
-  </si>
-  <si>
-    <t>yes_no</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>cadre_of_health_worker</t>
-  </si>
-  <si>
-    <t>Nurse</t>
-  </si>
-  <si>
-    <t>Clincal officer/Docter</t>
-  </si>
-  <si>
-    <t>Community health care worker</t>
-  </si>
-  <si>
-    <t>Employee</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>form_title</t>
-  </si>
-  <si>
-    <t>form_id</t>
-  </si>
-  <si>
-    <t>version</t>
-  </si>
-  <si>
-    <t>style</t>
-  </si>
-  <si>
-    <t>path</t>
-  </si>
-  <si>
-    <t>instance_name</t>
-  </si>
-  <si>
-    <t>HTS Linkage</t>
-  </si>
-  <si>
-    <t>hts_linkage</t>
-  </si>
-  <si>
-    <t>pages</t>
-  </si>
-  <si>
-    <t>data</t>
-  </si>
-  <si>
-    <t>_164401_otherCadre_99DCT</t>
-  </si>
-  <si>
-    <t>_162724_facilityLinkedTo_99DCT</t>
-  </si>
-  <si>
-    <t>_162053_cccNumber_99DCT</t>
-  </si>
-  <si>
-    <t>_1473_healthWorkerHandedTo_99DCT</t>
-  </si>
-  <si>
-    <t>_162577_cadreOfHealthWorker_99DCT</t>
-  </si>
-  <si>
-    <t>_160555_dateEnrolled_99DCT</t>
-  </si>
-  <si>
-    <t>_159599_ARTdate_99DCT</t>
-  </si>
-  <si>
-    <t>_163042_remarks_99DCT</t>
-  </si>
-  <si>
-    <t>_1577_nurse_99DCT</t>
-  </si>
-  <si>
-    <t>_1574_clinicalOficer_99DCT</t>
-  </si>
-  <si>
-    <t>_1555_communityHealthWorker_99DCT</t>
-  </si>
-  <si>
-    <t>_1540_employess_99DCT</t>
-  </si>
-  <si>
-    <t>_5622_other_99DCT</t>
-  </si>
-  <si>
-    <t>_1065_yes_99DCT</t>
-  </si>
-  <si>
-    <t>_1066_no_99DCT</t>
-  </si>
-  <si>
-    <t>_163137_encounterDAte_99DCT</t>
-  </si>
-  <si>
-    <t>${_162577_cadreOfHealthWorker_99DCT}=”_5622_other_99DCT”</t>
+    <t xml:space="preserve">_159599_ARTdate_99DCT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ART start date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_163042_remarks_99DCT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remark(s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">list_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes_no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_1065_yes_99DCT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_1066_no_99DCT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cadre_of_health_worker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_1577_nurse_99DCT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nurse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_1574_clinicalOficer_99DCT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clincal officer/Docter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_1555_communityHealthWorker_99DCT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Community health care worker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_1540_employess_99DCT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_5622_other_99DCT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">form_title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">form_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">style</t>
+  </si>
+  <si>
+    <t xml:space="preserve">path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">instance_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HTS Linkage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hts_linkage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy\ hh\-mm\-ss"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="DD\-MM\-YYYY\ HH\-MM\-SS"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFA9B7C6"/>
       <name val="DejaVu Sans Mono"/>
+      <family val="3"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF4C4C4C"/>
       <name val="Ubuntu"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFCCCCCC"/>
       <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Cambria"/>
+      <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Cambria"/>
     </font>
   </fonts>
   <fills count="4">
@@ -428,7 +444,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -436,69 +452,113 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+  <cellXfs count="16">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <dxfs count="26">
     <dxf>
       <font>
-        <color rgb="FFC27BA0"/>
+        <color rgb="FFB7B7B7"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFD9D2E9"/>
+          <bgColor rgb="FFD9EAD3"/>
         </patternFill>
       </fill>
     </dxf>
@@ -508,7 +568,55 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFD9D2E9"/>
+          <bgColor rgb="FFCFE2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC27BA0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCFE2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCCCCCC"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="1"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF980000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -520,141 +628,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <strike/>
-        <color rgb="FFFFFFFF"/>
-      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEAD1DC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -671,6 +647,138 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFEAD1DC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="1"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="1"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="1"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="1"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="1"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="1"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="1"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="1"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="1"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="1"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="1"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="1"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -684,39 +792,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FF76A5AF"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FF980000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFCCCCCC"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFD9D2E9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -726,32 +806,11 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFCFE2F3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF76A5AF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCFE2F3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFB7B7B7"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9D2E9"/>
         </patternFill>
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -810,352 +869,45 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF4C4C4C"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y1048576"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:Y65536"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C27" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="G5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="28.1328125" customWidth="1"/>
-    <col min="2" max="2" width="28.265625" customWidth="1"/>
-    <col min="3" max="3" width="48.53125" customWidth="1"/>
-    <col min="4" max="4" width="14.3984375" customWidth="1"/>
-    <col min="5" max="5" width="52.3984375" customWidth="1"/>
-    <col min="6" max="6" width="17.3984375" customWidth="1"/>
-    <col min="7" max="7" width="38.6640625" customWidth="1"/>
-    <col min="8" max="8" width="32.73046875" customWidth="1"/>
-    <col min="9" max="9" width="73.86328125" customWidth="1"/>
-    <col min="10" max="10" width="14.3984375" customWidth="1"/>
-    <col min="11" max="11" width="25.1328125" customWidth="1"/>
-    <col min="12" max="12" width="14.3984375" customWidth="1"/>
-    <col min="13" max="25" width="29.86328125" customWidth="1"/>
-    <col min="26" max="1025" width="14.3984375" customWidth="1"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.0663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.25"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.3061224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="54.265306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.9081632653061"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.9591836734694"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="33.8367346938776"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="76.4948979591837"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.9183673469388"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="25" min="13" style="0" width="30.8673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="14.8469387755102"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="13.9">
+    <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1208,7 +960,7 @@
       <c r="X1" s="2"/>
       <c r="Y1" s="2"/>
     </row>
-    <row r="2" spans="1:25" ht="13.5">
+    <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -1245,7 +997,7 @@
       <c r="X2" s="4"/>
       <c r="Y2" s="4"/>
     </row>
-    <row r="3" spans="1:25" ht="13.5">
+    <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -1280,7 +1032,7 @@
       <c r="X3" s="4"/>
       <c r="Y3" s="4"/>
     </row>
-    <row r="4" spans="1:25" ht="13.5">
+    <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
@@ -1313,7 +1065,7 @@
       <c r="X4" s="4"/>
       <c r="Y4" s="4"/>
     </row>
-    <row r="5" spans="1:25" ht="13.5">
+    <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -1346,7 +1098,7 @@
       <c r="X5" s="4"/>
       <c r="Y5" s="4"/>
     </row>
-    <row r="6" spans="1:25" ht="13.5">
+    <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>26</v>
       </c>
@@ -1381,7 +1133,7 @@
       <c r="X6" s="4"/>
       <c r="Y6" s="4"/>
     </row>
-    <row r="7" spans="1:25" ht="13.5">
+    <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -1414,7 +1166,7 @@
       <c r="X7" s="4"/>
       <c r="Y7" s="4"/>
     </row>
-    <row r="8" spans="1:25" ht="13.5">
+    <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
@@ -1447,7 +1199,7 @@
       <c r="X8" s="4"/>
       <c r="Y8" s="4"/>
     </row>
-    <row r="9" spans="1:25" ht="13.5">
+    <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
         <v>31</v>
       </c>
@@ -1482,7 +1234,7 @@
       <c r="X9" s="4"/>
       <c r="Y9" s="4"/>
     </row>
-    <row r="10" spans="1:25" ht="13.5">
+    <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
@@ -1515,7 +1267,7 @@
       <c r="X10" s="4"/>
       <c r="Y10" s="4"/>
     </row>
-    <row r="11" spans="1:25" ht="13.5">
+    <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
         <v>34</v>
       </c>
@@ -1544,7 +1296,7 @@
       <c r="X11" s="4"/>
       <c r="Y11" s="4"/>
     </row>
-    <row r="12" spans="1:25" ht="13.5">
+    <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
@@ -1577,7 +1329,7 @@
       <c r="X12" s="4"/>
       <c r="Y12" s="4"/>
     </row>
-    <row r="13" spans="1:25" ht="13.5">
+    <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
@@ -1610,7 +1362,7 @@
       <c r="X13" s="4"/>
       <c r="Y13" s="4"/>
     </row>
-    <row r="14" spans="1:25" ht="13.5">
+    <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -1643,7 +1395,7 @@
       <c r="X14" s="4"/>
       <c r="Y14" s="4"/>
     </row>
-    <row r="15" spans="1:25" ht="13.5">
+    <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
         <v>18</v>
       </c>
@@ -1676,7 +1428,7 @@
       <c r="X15" s="4"/>
       <c r="Y15" s="4"/>
     </row>
-    <row r="16" spans="1:25" ht="13.5">
+    <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
@@ -1709,7 +1461,7 @@
       <c r="X16" s="4"/>
       <c r="Y16" s="4"/>
     </row>
-    <row r="17" spans="1:25" ht="13.5">
+    <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
         <v>34</v>
       </c>
@@ -1738,7 +1490,7 @@
       <c r="X17" s="4"/>
       <c r="Y17" s="4"/>
     </row>
-    <row r="18" spans="1:25" ht="13.5">
+    <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
         <v>34</v>
       </c>
@@ -1767,7 +1519,7 @@
       <c r="X18" s="4"/>
       <c r="Y18" s="4"/>
     </row>
-    <row r="19" spans="1:25" ht="13.5">
+    <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
         <v>34</v>
       </c>
@@ -1796,7 +1548,7 @@
       <c r="X19" s="4"/>
       <c r="Y19" s="4"/>
     </row>
-    <row r="20" spans="1:25" ht="13.5">
+    <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
         <v>34</v>
       </c>
@@ -1825,7 +1577,7 @@
       <c r="X20" s="4"/>
       <c r="Y20" s="4"/>
     </row>
-    <row r="21" spans="1:25" ht="13.5">
+    <row r="21" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
         <v>34</v>
       </c>
@@ -1854,7 +1606,7 @@
       <c r="X21" s="4"/>
       <c r="Y21" s="4"/>
     </row>
-    <row r="22" spans="1:25" ht="13.5">
+    <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
         <v>40</v>
       </c>
@@ -1889,7 +1641,7 @@
       <c r="X22" s="4"/>
       <c r="Y22" s="4"/>
     </row>
-    <row r="23" spans="1:25" ht="13.5">
+    <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
         <v>40</v>
       </c>
@@ -1924,7 +1676,7 @@
       <c r="X23" s="4"/>
       <c r="Y23" s="4"/>
     </row>
-    <row r="24" spans="1:25" ht="13.5">
+    <row r="24" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
         <v>40</v>
       </c>
@@ -1959,7 +1711,7 @@
       <c r="X24" s="5"/>
       <c r="Y24" s="5"/>
     </row>
-    <row r="25" spans="1:25" ht="13.5">
+    <row r="25" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
         <v>40</v>
       </c>
@@ -1994,7 +1746,7 @@
       <c r="X25" s="5"/>
       <c r="Y25" s="5"/>
     </row>
-    <row r="26" spans="1:25" ht="13.5">
+    <row r="26" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
         <v>40</v>
       </c>
@@ -2029,24 +1781,24 @@
       <c r="X26" s="5"/>
       <c r="Y26" s="5"/>
     </row>
-    <row r="27" spans="1:25" ht="13.5">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="6" t="s">
-        <v>51</v>
+      <c r="C27" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
-      <c r="F27" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
+      <c r="I27" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
@@ -2064,24 +1816,24 @@
       <c r="X27" s="5"/>
       <c r="Y27" s="5"/>
     </row>
-    <row r="28" spans="1:25" ht="13.5">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>54</v>
-      </c>
+      <c r="C28" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
+      <c r="I28" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
@@ -2099,21 +1851,21 @@
       <c r="X28" s="5"/>
       <c r="Y28" s="5"/>
     </row>
-    <row r="29" spans="1:25" ht="27">
+    <row r="29" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>54</v>
-      </c>
+      <c r="D29" s="5"/>
       <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
+      <c r="F29" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
@@ -2134,23 +1886,23 @@
       <c r="X29" s="5"/>
       <c r="Y29" s="5"/>
     </row>
-    <row r="30" spans="1:25" ht="13.5">
+    <row r="30" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C30" s="5" t="s">
         <v>57</v>
       </c>
+      <c r="C30" s="7" t="s">
+        <v>58</v>
+      </c>
       <c r="D30" s="5" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
@@ -2169,23 +1921,23 @@
       <c r="X30" s="5"/>
       <c r="Y30" s="5"/>
     </row>
-    <row r="31" spans="1:25" ht="27">
+    <row r="31" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
@@ -2204,17 +1956,19 @@
       <c r="X31" s="5"/>
       <c r="Y31" s="5"/>
     </row>
-    <row r="32" spans="1:25" ht="27">
+    <row r="32" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
@@ -2237,10 +1991,16 @@
       <c r="X32" s="5"/>
       <c r="Y32" s="5"/>
     </row>
-    <row r="33" spans="1:25" ht="13.5">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
+    <row r="33" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>66</v>
+      </c>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
@@ -2264,20 +2024,12 @@
       <c r="X33" s="5"/>
       <c r="Y33" s="5"/>
     </row>
-    <row r="34" spans="1:25" ht="27">
-      <c r="A34" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>61</v>
-      </c>
+    <row r="34" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
       <c r="D34" s="5"/>
-      <c r="E34" s="8" t="s">
-        <v>101</v>
-      </c>
+      <c r="E34" s="5"/>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
@@ -2299,12 +2051,20 @@
       <c r="X34" s="5"/>
       <c r="Y34" s="5"/>
     </row>
-    <row r="35" spans="1:25" ht="13.5">
-      <c r="A35" s="5"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
+    <row r="35" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
+      <c r="E35" s="8" t="s">
+        <v>69</v>
+      </c>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
@@ -2326,23 +2086,15 @@
       <c r="X35" s="5"/>
       <c r="Y35" s="5"/>
     </row>
-    <row r="36" spans="1:25" ht="13.5">
-      <c r="A36" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>54</v>
-      </c>
+    <row r="36" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
@@ -2361,18 +2113,18 @@
       <c r="X36" s="5"/>
       <c r="Y36" s="5"/>
     </row>
-    <row r="37" spans="1:25" ht="13.5">
+    <row r="37" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
@@ -2396,17 +2148,19 @@
       <c r="X37" s="5"/>
       <c r="Y37" s="5"/>
     </row>
-    <row r="38" spans="1:25" ht="13.5">
+    <row r="38" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D38" s="5"/>
+        <v>74</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
       <c r="G38" s="4"/>
@@ -2429,10 +2183,16 @@
       <c r="X38" s="5"/>
       <c r="Y38" s="5"/>
     </row>
-    <row r="39" spans="1:25" ht="13.5">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
+    <row r="39" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>76</v>
+      </c>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
@@ -2456,15 +2216,15 @@
       <c r="X39" s="5"/>
       <c r="Y39" s="5"/>
     </row>
-    <row r="40" spans="1:25" ht="13.5">
+    <row r="40" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
-      <c r="H40" s="5"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
       <c r="K40" s="5"/>
@@ -2483,10 +2243,8 @@
       <c r="X40" s="5"/>
       <c r="Y40" s="5"/>
     </row>
-    <row r="41" spans="1:25" ht="13.5">
-      <c r="A41" s="5" t="s">
-        <v>34</v>
-      </c>
+    <row r="41" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
@@ -2512,8 +2270,10 @@
       <c r="X41" s="5"/>
       <c r="Y41" s="5"/>
     </row>
-    <row r="42" spans="1:25" ht="13.5">
-      <c r="A42" s="4"/>
+    <row r="42" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
@@ -2539,7 +2299,7 @@
       <c r="X42" s="5"/>
       <c r="Y42" s="5"/>
     </row>
-    <row r="43" spans="1:25" ht="13.5">
+    <row r="43" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -2566,10 +2326,10 @@
       <c r="X43" s="5"/>
       <c r="Y43" s="5"/>
     </row>
-    <row r="44" spans="1:25" ht="13.5">
+    <row r="44" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="4"/>
       <c r="B44" s="5"/>
-      <c r="C44" s="7"/>
+      <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
@@ -2593,7 +2353,7 @@
       <c r="X44" s="5"/>
       <c r="Y44" s="5"/>
     </row>
-    <row r="45" spans="1:25" ht="13.5">
+    <row r="45" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4"/>
       <c r="B45" s="5"/>
       <c r="C45" s="7"/>
@@ -2620,10 +2380,10 @@
       <c r="X45" s="5"/>
       <c r="Y45" s="5"/>
     </row>
-    <row r="46" spans="1:25" ht="13.5">
+    <row r="46" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="4"/>
       <c r="B46" s="5"/>
-      <c r="C46" s="5"/>
+      <c r="C46" s="7"/>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
@@ -2647,36 +2407,36 @@
       <c r="X46" s="5"/>
       <c r="Y46" s="5"/>
     </row>
-    <row r="47" spans="1:25" ht="13.5">
+    <row r="47" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="4"/>
-      <c r="B47" s="9"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
-      <c r="H47" s="4"/>
-      <c r="I47" s="4"/>
-      <c r="J47" s="4"/>
-      <c r="K47" s="4"/>
-      <c r="L47" s="4"/>
-      <c r="M47" s="4"/>
-      <c r="N47" s="4"/>
-      <c r="O47" s="4"/>
-      <c r="P47" s="4"/>
-      <c r="Q47" s="4"/>
-      <c r="R47" s="4"/>
-      <c r="S47" s="4"/>
-      <c r="T47" s="4"/>
-      <c r="U47" s="4"/>
-      <c r="V47" s="4"/>
-      <c r="W47" s="4"/>
-      <c r="X47" s="4"/>
-      <c r="Y47" s="4"/>
-    </row>
-    <row r="48" spans="1:25" ht="13.5">
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="5"/>
+      <c r="M47" s="5"/>
+      <c r="N47" s="5"/>
+      <c r="O47" s="5"/>
+      <c r="P47" s="5"/>
+      <c r="Q47" s="5"/>
+      <c r="R47" s="5"/>
+      <c r="S47" s="5"/>
+      <c r="T47" s="5"/>
+      <c r="U47" s="5"/>
+      <c r="V47" s="5"/>
+      <c r="W47" s="5"/>
+      <c r="X47" s="5"/>
+      <c r="Y47" s="5"/>
+    </row>
+    <row r="48" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="4"/>
-      <c r="B48" s="4"/>
+      <c r="B48" s="9"/>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
@@ -2701,7 +2461,7 @@
       <c r="X48" s="4"/>
       <c r="Y48" s="4"/>
     </row>
-    <row r="49" spans="1:25" ht="13.5">
+    <row r="49" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
@@ -2728,7 +2488,7 @@
       <c r="X49" s="4"/>
       <c r="Y49" s="4"/>
     </row>
-    <row r="50" spans="1:25" ht="13.5">
+    <row r="50" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -2755,7 +2515,7 @@
       <c r="X50" s="4"/>
       <c r="Y50" s="4"/>
     </row>
-    <row r="51" spans="1:25" ht="13.5">
+    <row r="51" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -2782,88 +2542,88 @@
       <c r="X51" s="4"/>
       <c r="Y51" s="4"/>
     </row>
-    <row r="52" spans="1:25" ht="13.5">
-      <c r="A52" s="5"/>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5"/>
-      <c r="F52" s="5"/>
-      <c r="G52" s="5"/>
-      <c r="H52" s="5"/>
-      <c r="I52" s="5"/>
-      <c r="J52" s="5"/>
-      <c r="K52" s="5"/>
-      <c r="L52" s="5"/>
-      <c r="M52" s="5"/>
-      <c r="N52" s="5"/>
-      <c r="O52" s="5"/>
-      <c r="P52" s="5"/>
-      <c r="Q52" s="5"/>
-      <c r="R52" s="5"/>
-      <c r="S52" s="5"/>
-      <c r="T52" s="5"/>
-      <c r="U52" s="5"/>
-      <c r="V52" s="5"/>
-      <c r="W52" s="5"/>
-      <c r="X52" s="5"/>
-      <c r="Y52" s="5"/>
-    </row>
-    <row r="53" spans="1:25" ht="13.5">
-      <c r="A53" s="4"/>
-      <c r="B53" s="4"/>
-      <c r="C53" s="7"/>
-      <c r="D53" s="4"/>
-      <c r="E53" s="4"/>
-      <c r="F53" s="4"/>
-      <c r="G53" s="4"/>
-      <c r="H53" s="4"/>
-      <c r="I53" s="4"/>
-      <c r="J53" s="4"/>
-      <c r="K53" s="4"/>
-      <c r="L53" s="4"/>
-      <c r="M53" s="4"/>
-      <c r="N53" s="4"/>
-      <c r="O53" s="4"/>
-      <c r="P53" s="4"/>
-      <c r="Q53" s="4"/>
-      <c r="R53" s="4"/>
-      <c r="S53" s="4"/>
-      <c r="T53" s="4"/>
-      <c r="U53" s="4"/>
-      <c r="V53" s="4"/>
-      <c r="W53" s="4"/>
-      <c r="X53" s="4"/>
-      <c r="Y53" s="4"/>
-    </row>
-    <row r="54" spans="1:25" ht="13.5">
+    <row r="52" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="4"/>
+      <c r="K52" s="4"/>
+      <c r="L52" s="4"/>
+      <c r="M52" s="4"/>
+      <c r="N52" s="4"/>
+      <c r="O52" s="4"/>
+      <c r="P52" s="4"/>
+      <c r="Q52" s="4"/>
+      <c r="R52" s="4"/>
+      <c r="S52" s="4"/>
+      <c r="T52" s="4"/>
+      <c r="U52" s="4"/>
+      <c r="V52" s="4"/>
+      <c r="W52" s="4"/>
+      <c r="X52" s="4"/>
+      <c r="Y52" s="4"/>
+    </row>
+    <row r="53" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="5"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="5"/>
+      <c r="J53" s="5"/>
+      <c r="K53" s="5"/>
+      <c r="L53" s="5"/>
+      <c r="M53" s="5"/>
+      <c r="N53" s="5"/>
+      <c r="O53" s="5"/>
+      <c r="P53" s="5"/>
+      <c r="Q53" s="5"/>
+      <c r="R53" s="5"/>
+      <c r="S53" s="5"/>
+      <c r="T53" s="5"/>
+      <c r="U53" s="5"/>
+      <c r="V53" s="5"/>
+      <c r="W53" s="5"/>
+      <c r="X53" s="5"/>
+      <c r="Y53" s="5"/>
+    </row>
+    <row r="54" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="4"/>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="4"/>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
-      <c r="G54" s="5"/>
-      <c r="H54" s="5"/>
-      <c r="I54" s="5"/>
-      <c r="J54" s="5"/>
-      <c r="K54" s="5"/>
-      <c r="L54" s="5"/>
-      <c r="M54" s="5"/>
-      <c r="N54" s="5"/>
-      <c r="O54" s="5"/>
-      <c r="P54" s="5"/>
-      <c r="Q54" s="5"/>
-      <c r="R54" s="5"/>
-      <c r="S54" s="5"/>
-      <c r="T54" s="5"/>
-      <c r="U54" s="5"/>
-      <c r="V54" s="5"/>
-      <c r="W54" s="5"/>
-      <c r="X54" s="5"/>
-      <c r="Y54" s="5"/>
-    </row>
-    <row r="55" spans="1:25" ht="13.5">
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="4"/>
+      <c r="J54" s="4"/>
+      <c r="K54" s="4"/>
+      <c r="L54" s="4"/>
+      <c r="M54" s="4"/>
+      <c r="N54" s="4"/>
+      <c r="O54" s="4"/>
+      <c r="P54" s="4"/>
+      <c r="Q54" s="4"/>
+      <c r="R54" s="4"/>
+      <c r="S54" s="4"/>
+      <c r="T54" s="4"/>
+      <c r="U54" s="4"/>
+      <c r="V54" s="4"/>
+      <c r="W54" s="4"/>
+      <c r="X54" s="4"/>
+      <c r="Y54" s="4"/>
+    </row>
+    <row r="55" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="4"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
@@ -2890,13 +2650,13 @@
       <c r="X55" s="5"/>
       <c r="Y55" s="5"/>
     </row>
-    <row r="56" spans="1:25" ht="13.5">
-      <c r="A56" s="5"/>
+    <row r="56" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="4"/>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
-      <c r="E56" s="5"/>
-      <c r="F56" s="5"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
       <c r="G56" s="5"/>
       <c r="H56" s="5"/>
       <c r="I56" s="5"/>
@@ -2917,146 +2677,146 @@
       <c r="X56" s="5"/>
       <c r="Y56" s="5"/>
     </row>
-    <row r="57" spans="1:25" ht="13.5">
-      <c r="A57" s="4"/>
-      <c r="B57" s="4"/>
-      <c r="C57" s="4"/>
-      <c r="D57" s="4"/>
-      <c r="E57" s="4"/>
-      <c r="F57" s="4"/>
-      <c r="G57" s="4"/>
-      <c r="H57" s="4"/>
-      <c r="I57" s="4"/>
-      <c r="J57" s="4"/>
-      <c r="K57" s="4"/>
-      <c r="L57" s="4"/>
-      <c r="M57" s="4"/>
-      <c r="N57" s="4"/>
-      <c r="O57" s="4"/>
-      <c r="P57" s="4"/>
-      <c r="Q57" s="4"/>
-      <c r="R57" s="4"/>
-      <c r="S57" s="4"/>
-      <c r="T57" s="4"/>
-      <c r="U57" s="4"/>
-      <c r="V57" s="4"/>
-      <c r="W57" s="4"/>
-      <c r="X57" s="4"/>
-      <c r="Y57" s="4"/>
-    </row>
-    <row r="58" spans="1:25" ht="13.5">
+    <row r="57" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="5"/>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="5"/>
+      <c r="I57" s="5"/>
+      <c r="J57" s="5"/>
+      <c r="K57" s="5"/>
+      <c r="L57" s="5"/>
+      <c r="M57" s="5"/>
+      <c r="N57" s="5"/>
+      <c r="O57" s="5"/>
+      <c r="P57" s="5"/>
+      <c r="Q57" s="5"/>
+      <c r="R57" s="5"/>
+      <c r="S57" s="5"/>
+      <c r="T57" s="5"/>
+      <c r="U57" s="5"/>
+      <c r="V57" s="5"/>
+      <c r="W57" s="5"/>
+      <c r="X57" s="5"/>
+      <c r="Y57" s="5"/>
+    </row>
+    <row r="58" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="4"/>
-      <c r="B58" s="5"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="4"/>
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
-      <c r="G58" s="5"/>
-      <c r="H58" s="5"/>
-      <c r="I58" s="5"/>
-      <c r="J58" s="5"/>
-      <c r="K58" s="5"/>
-      <c r="L58" s="5"/>
-      <c r="M58" s="5"/>
-      <c r="N58" s="5"/>
-      <c r="O58" s="5"/>
-      <c r="P58" s="5"/>
-      <c r="Q58" s="5"/>
-      <c r="R58" s="5"/>
-      <c r="S58" s="5"/>
-      <c r="T58" s="5"/>
-      <c r="U58" s="5"/>
-      <c r="V58" s="5"/>
-      <c r="W58" s="5"/>
-      <c r="X58" s="5"/>
-      <c r="Y58" s="5"/>
-    </row>
-    <row r="59" spans="1:25" ht="13.5">
+      <c r="G58" s="4"/>
+      <c r="H58" s="4"/>
+      <c r="I58" s="4"/>
+      <c r="J58" s="4"/>
+      <c r="K58" s="4"/>
+      <c r="L58" s="4"/>
+      <c r="M58" s="4"/>
+      <c r="N58" s="4"/>
+      <c r="O58" s="4"/>
+      <c r="P58" s="4"/>
+      <c r="Q58" s="4"/>
+      <c r="R58" s="4"/>
+      <c r="S58" s="4"/>
+      <c r="T58" s="4"/>
+      <c r="U58" s="4"/>
+      <c r="V58" s="4"/>
+      <c r="W58" s="4"/>
+      <c r="X58" s="4"/>
+      <c r="Y58" s="4"/>
+    </row>
+    <row r="59" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="4"/>
-      <c r="B59" s="4"/>
-      <c r="C59" s="4"/>
-      <c r="D59" s="4"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
-      <c r="G59" s="4"/>
-      <c r="H59" s="4"/>
-      <c r="I59" s="4"/>
-      <c r="J59" s="4"/>
-      <c r="K59" s="4"/>
-      <c r="L59" s="4"/>
-      <c r="M59" s="4"/>
-      <c r="N59" s="4"/>
-      <c r="O59" s="4"/>
-      <c r="P59" s="4"/>
-      <c r="Q59" s="4"/>
-      <c r="R59" s="4"/>
-      <c r="S59" s="4"/>
-      <c r="T59" s="4"/>
-      <c r="U59" s="4"/>
-      <c r="V59" s="4"/>
-      <c r="W59" s="4"/>
-      <c r="X59" s="4"/>
-      <c r="Y59" s="4"/>
-    </row>
-    <row r="60" spans="1:25" ht="13.5">
-      <c r="A60" s="5"/>
-      <c r="B60" s="5"/>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
-      <c r="E60" s="5"/>
-      <c r="F60" s="5"/>
-      <c r="G60" s="5"/>
-      <c r="H60" s="5"/>
-      <c r="I60" s="5"/>
-      <c r="J60" s="5"/>
-      <c r="K60" s="5"/>
-      <c r="L60" s="5"/>
-      <c r="M60" s="5"/>
-      <c r="N60" s="5"/>
-      <c r="O60" s="5"/>
-      <c r="P60" s="5"/>
-      <c r="Q60" s="5"/>
-      <c r="R60" s="5"/>
-      <c r="S60" s="5"/>
-      <c r="T60" s="5"/>
-      <c r="U60" s="5"/>
-      <c r="V60" s="5"/>
-      <c r="W60" s="5"/>
-      <c r="X60" s="5"/>
-      <c r="Y60" s="5"/>
-    </row>
-    <row r="61" spans="1:25" ht="13.5">
-      <c r="A61" s="10"/>
-      <c r="B61" s="4"/>
-      <c r="C61" s="4"/>
-      <c r="D61" s="4"/>
-      <c r="E61" s="4"/>
-      <c r="F61" s="4"/>
-      <c r="G61" s="11"/>
-      <c r="H61" s="11"/>
-      <c r="I61" s="11"/>
-      <c r="J61" s="11"/>
-      <c r="K61" s="11"/>
-      <c r="L61" s="11"/>
-      <c r="M61" s="11"/>
-      <c r="N61" s="11"/>
-      <c r="O61" s="11"/>
-      <c r="P61" s="11"/>
-      <c r="Q61" s="11"/>
-      <c r="R61" s="11"/>
-      <c r="S61" s="11"/>
-      <c r="T61" s="11"/>
-      <c r="U61" s="11"/>
-      <c r="V61" s="11"/>
-      <c r="W61" s="11"/>
-      <c r="X61" s="11"/>
-      <c r="Y61" s="11"/>
-    </row>
-    <row r="62" spans="1:25" ht="13.5">
+      <c r="G59" s="5"/>
+      <c r="H59" s="5"/>
+      <c r="I59" s="5"/>
+      <c r="J59" s="5"/>
+      <c r="K59" s="5"/>
+      <c r="L59" s="5"/>
+      <c r="M59" s="5"/>
+      <c r="N59" s="5"/>
+      <c r="O59" s="5"/>
+      <c r="P59" s="5"/>
+      <c r="Q59" s="5"/>
+      <c r="R59" s="5"/>
+      <c r="S59" s="5"/>
+      <c r="T59" s="5"/>
+      <c r="U59" s="5"/>
+      <c r="V59" s="5"/>
+      <c r="W59" s="5"/>
+      <c r="X59" s="5"/>
+      <c r="Y59" s="5"/>
+    </row>
+    <row r="60" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="4"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="4"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="4"/>
+      <c r="J60" s="4"/>
+      <c r="K60" s="4"/>
+      <c r="L60" s="4"/>
+      <c r="M60" s="4"/>
+      <c r="N60" s="4"/>
+      <c r="O60" s="4"/>
+      <c r="P60" s="4"/>
+      <c r="Q60" s="4"/>
+      <c r="R60" s="4"/>
+      <c r="S60" s="4"/>
+      <c r="T60" s="4"/>
+      <c r="U60" s="4"/>
+      <c r="V60" s="4"/>
+      <c r="W60" s="4"/>
+      <c r="X60" s="4"/>
+      <c r="Y60" s="4"/>
+    </row>
+    <row r="61" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="5"/>
+      <c r="B61" s="5"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
+      <c r="G61" s="5"/>
+      <c r="H61" s="5"/>
+      <c r="I61" s="5"/>
+      <c r="J61" s="5"/>
+      <c r="K61" s="5"/>
+      <c r="L61" s="5"/>
+      <c r="M61" s="5"/>
+      <c r="N61" s="5"/>
+      <c r="O61" s="5"/>
+      <c r="P61" s="5"/>
+      <c r="Q61" s="5"/>
+      <c r="R61" s="5"/>
+      <c r="S61" s="5"/>
+      <c r="T61" s="5"/>
+      <c r="U61" s="5"/>
+      <c r="V61" s="5"/>
+      <c r="W61" s="5"/>
+      <c r="X61" s="5"/>
+      <c r="Y61" s="5"/>
+    </row>
+    <row r="62" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="10"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
-      <c r="D62" s="11"/>
+      <c r="D62" s="4"/>
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
       <c r="G62" s="11"/>
@@ -3079,7 +2839,7 @@
       <c r="X62" s="11"/>
       <c r="Y62" s="11"/>
     </row>
-    <row r="63" spans="1:25" ht="13.5">
+    <row r="63" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="10"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
@@ -3106,161 +2866,197 @@
       <c r="X63" s="11"/>
       <c r="Y63" s="11"/>
     </row>
-    <row r="1048576" ht="15.75" customHeight="1"/>
+    <row r="64" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="10"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="4"/>
+      <c r="D64" s="11"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4"/>
+      <c r="G64" s="11"/>
+      <c r="H64" s="11"/>
+      <c r="I64" s="11"/>
+      <c r="J64" s="11"/>
+      <c r="K64" s="11"/>
+      <c r="L64" s="11"/>
+      <c r="M64" s="11"/>
+      <c r="N64" s="11"/>
+      <c r="O64" s="11"/>
+      <c r="P64" s="11"/>
+      <c r="Q64" s="11"/>
+      <c r="R64" s="11"/>
+      <c r="S64" s="11"/>
+      <c r="T64" s="11"/>
+      <c r="U64" s="11"/>
+      <c r="V64" s="11"/>
+      <c r="W64" s="11"/>
+      <c r="X64" s="11"/>
+      <c r="Y64" s="11"/>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <conditionalFormatting sqref="A1:Y1019">
-    <cfRule type="containsText" dxfId="25" priority="2" operator="containsText" text="calculate"/>
+  <conditionalFormatting sqref="A1:Y26,A29:Y1020">
+    <cfRule type="containsText" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:Y1004">
-    <cfRule type="expression" dxfId="24" priority="3">
+  <conditionalFormatting sqref="A1:Y26,A29:Y1005">
+    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A1="begin group", NOT($B1 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:Y1019">
-    <cfRule type="expression" dxfId="23" priority="4">
+  <conditionalFormatting sqref="A1:Y26,A29:Y1020">
+    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>AND($A1="end group", $B1 = "", $C1 = "", $D1 = "", $E1 = "", $F1 = "", $G1 = "", $H1 = "", $I1 = "", $J1 = "", $K1 = "", $L1 = "", $M1 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:Y1019">
-    <cfRule type="cellIs" dxfId="22" priority="5" operator="equal">
+  <conditionalFormatting sqref="A1:Y26,A29:Y1020">
+    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="expression" dxfId="21" priority="6">
-      <formula>AND(A1 = "type", COUNTIF($A$1:$A$1013, "begin group") = COUNTIF($A$1:$A$1013, "end group"))</formula>
+    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>AND(A1 = "type", COUNTIF($A$1:$A$1014, "begin group") = COUNTIF($A$1:$A$1014, "end group"))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="expression" dxfId="20" priority="7">
-      <formula>OR(NOT(A1 = "type"), NOT(COUNTIF($A$1:$A$1004, "begin group") = COUNTIF($A$1:$A$1013, "end group")))</formula>
+    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>OR(NOT(A1 = "type"), NOT(COUNTIF($A$1:$A$1005, "begin group") = COUNTIF($A$1:$A$1014, "end group")))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I1:I1019">
-    <cfRule type="expression" dxfId="19" priority="8">
+  <conditionalFormatting sqref="I1:I26,I29:I1020">
+    <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($I1 = "", $A1 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C1019">
-    <cfRule type="expression" dxfId="18" priority="9">
+  <conditionalFormatting sqref="C1:C26,C29:C1020">
+    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND(AND(NOT($A1 = "end group"), NOT($A1 = "end repeat"), NOT($A1 = "")), $C1 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1019">
-    <cfRule type="expression" dxfId="17" priority="10">
+  <conditionalFormatting sqref="B1:B26,B29:B1020">
+    <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>AND(AND(NOT($A1 = "end group"), NOT($A1 = "end repeat"), NOT($A1 = "")), $B1 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A1019">
-    <cfRule type="cellIs" dxfId="16" priority="11" operator="equal">
+  <conditionalFormatting sqref="A1:A26,A29:A1020">
+    <cfRule type="cellIs" priority="11" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B1012">
-    <cfRule type="expression" dxfId="15" priority="12">
-      <formula>COUNTIF($B$2:$B$1012,B2)&gt;1</formula>
+  <conditionalFormatting sqref="B2:B26,B29:B1013">
+    <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+      <formula>COUNTIF($B$2:$B$1013,B2)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1">
-    <cfRule type="cellIs" dxfId="14" priority="13" operator="notEqual">
+    <cfRule type="cellIs" priority="13" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>"name"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1">
-    <cfRule type="notContainsText" dxfId="13" priority="14" operator="notContains" text="label"/>
+    <cfRule type="notContainsText" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="label" dxfId="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1">
-    <cfRule type="cellIs" dxfId="12" priority="15" operator="notEqual">
+    <cfRule type="cellIs" priority="15" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
       <formula>"required"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1">
-    <cfRule type="cellIs" dxfId="11" priority="16" operator="notEqual">
+    <cfRule type="cellIs" priority="16" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
       <formula>"relevant"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="cellIs" dxfId="10" priority="17" operator="notEqual">
+    <cfRule type="cellIs" priority="17" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
       <formula>"appearance"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1">
-    <cfRule type="cellIs" dxfId="9" priority="18" operator="notEqual">
+    <cfRule type="cellIs" priority="18" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
       <formula>"constraint"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="notContainsText" dxfId="8" priority="19" operator="notContains" text="constraint_message"/>
+    <cfRule type="notContainsText" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="constraint_message" dxfId="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1">
-    <cfRule type="cellIs" dxfId="7" priority="20" operator="notEqual">
+    <cfRule type="cellIs" priority="20" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18">
       <formula>"calculation"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1">
-    <cfRule type="cellIs" dxfId="6" priority="21" operator="notEqual">
+    <cfRule type="cellIs" priority="21" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19">
       <formula>"choice_filter"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1">
-    <cfRule type="notContainsText" dxfId="5" priority="22" operator="notContains" text="hint"/>
+    <cfRule type="notContainsText" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="hint" dxfId="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1">
-    <cfRule type="cellIs" dxfId="4" priority="23" operator="notEqual">
+    <cfRule type="cellIs" priority="23" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21">
       <formula>"default"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:Y1">
-    <cfRule type="cellIs" dxfId="3" priority="24" operator="notEqual">
+    <cfRule type="cellIs" priority="24" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22">
       <formula>"media::image"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H1004">
-    <cfRule type="expression" dxfId="2" priority="25">
+  <conditionalFormatting sqref="H1:H26,H29:H1005">
+    <cfRule type="expression" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23">
       <formula>AND(NOT($G1 = ""), $H1 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:Y1004">
-    <cfRule type="expression" dxfId="1" priority="26">
+  <conditionalFormatting sqref="A1:Y26,A29:Y1005">
+    <cfRule type="expression" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24">
       <formula>AND($A1="begin repeat", NOT($B1 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:Y1019">
-    <cfRule type="expression" dxfId="0" priority="27">
+  <conditionalFormatting sqref="A1:Y26,A29:Y1020">
+    <cfRule type="expression" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25">
       <formula>AND($A1="end repeat", $B1 = "", $C1 = "", $D1 = "", $E1 = "", $F1 = "", $G1 = "", $H1 = "", $I1 = "", $J1 = "", $K1 = "", $L1 = "", $M1 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="D2:D63" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D2:D64" type="list">
       <formula1>"yes,no"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F1048576"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F65536"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="25.53125" customWidth="1"/>
-    <col min="2" max="2" width="31.1328125" customWidth="1"/>
-    <col min="3" max="3" width="39.1328125" customWidth="1"/>
-    <col min="4" max="1025" width="14.3984375" customWidth="1"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.219387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.5"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="14.8469387755102"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13.9">
+    <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>1</v>
@@ -3272,35 +3068,35 @@
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
     </row>
-    <row r="2" spans="1:6" ht="13.5">
+    <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="D2" s="14"/>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
     </row>
-    <row r="3" spans="1:6" ht="13.5">
+    <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
       <c r="F3" s="14"/>
     </row>
-    <row r="4" spans="1:6" ht="13.5">
+    <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="14"/>
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
@@ -3308,141 +3104,155 @@
       <c r="E4" s="14"/>
       <c r="F4" s="14"/>
     </row>
-    <row r="5" spans="1:6" ht="13.5">
+    <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="14"/>
       <c r="F5" s="14"/>
     </row>
-    <row r="6" spans="1:6" ht="13.5">
+    <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="14" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
     </row>
-    <row r="7" spans="1:6" ht="27">
+    <row r="7" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="14" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
     </row>
-    <row r="8" spans="1:6" ht="13.5">
-      <c r="A8" s="15" t="s">
-        <v>69</v>
+    <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="14" t="s">
+        <v>83</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
     </row>
-    <row r="9" spans="1:6" ht="13.5">
-      <c r="A9" s="15" t="s">
-        <v>69</v>
+    <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="14" t="s">
+        <v>83</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>74</v>
+        <v>93</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
     </row>
-    <row r="1048576" ht="15.75" customHeight="1"/>
+    <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F1048576"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F65536"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" width="14.3984375" customWidth="1"/>
-    <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="1025" width="14.3984375" customWidth="1"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="14.8469387755102"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="27.75">
+    <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="13.5">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="C2" s="16">
-        <f ca="1">NOW()</f>
-        <v>44054.403139699076</v>
+        <v>101</v>
+      </c>
+      <c r="C2" s="15" t="n">
+        <f aca="true">NOW()</f>
+        <v>44056.7421792928</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>83</v>
+        <v>102</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="F2" s="14"/>
     </row>
-    <row r="1048576" ht="15.75" customHeight="1"/>
+    <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
validated hts initial and retest forms. prepopulated forms with previously entered data
</commit_message>
<xml_diff>
--- a/config/default/forms/app/hts_linkage.xlsx
+++ b/config/default/forms/app/hts_linkage.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="108">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -186,7 +186,25 @@
     <t xml:space="preserve">'9c0a7a57-62ff-4f75-babe-5835b0e921b7'</t>
   </si>
   <si>
-    <t xml:space="preserve">observation</t>
+    <t xml:space="preserve">date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">encounter_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date of linkage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">floor(decimal-date-time(.)) &lt;= floor(decimal-date-time(today())) and floor( difference-in-months( . , today() ) div 12 ) &lt;= 100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Encounter date can not be in the future</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hts_linkage_assessment</t>
   </si>
   <si>
     <t xml:space="preserve">Linkage to care</t>
@@ -201,9 +219,6 @@
     <t xml:space="preserve">Facility linked to:  </t>
   </si>
   <si>
-    <t xml:space="preserve">yes</t>
-  </si>
-  <si>
     <t xml:space="preserve">_162053_cccNumber_99DCT</t>
   </si>
   <si>
@@ -232,9 +247,6 @@
   </si>
   <si>
     <t xml:space="preserve">${_162577_cadreOfHealthWorker_99DCT}=”_5622_other_99DCT”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date</t>
   </si>
   <si>
     <t xml:space="preserve">_160555_dateEnrolled_99DCT</t>
@@ -551,7 +563,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="38">
     <dxf>
       <font>
         <color rgb="FFB7B7B7"/>
@@ -807,6 +819,114 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFD9D2E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF76A5AF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCFE2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC27BA0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCFE2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF76A5AF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD9D2E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC27BA0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD9D2E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF980000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEAD1DC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFB7B7B7"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCCCCCC"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCCCCCC"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFF2CC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -879,32 +999,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y65536"/>
+  <dimension ref="A1:Y66"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="G5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="I28" activeCellId="0" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.0663265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.25"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.3061224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="54.265306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.9081632653061"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.9591836734694"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="33.8367346938776"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="76.4948979591837"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.9183673469388"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="25" min="13" style="0" width="30.8673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.1479591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.3265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.015306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.3010204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="56.2448979591837"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.5408163265306"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.3979591836735"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="35.0102040816326"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="79.1938775510204"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.3010204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="26.8163265306122"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.3010204081633"/>
+    <col collapsed="false" hidden="false" max="25" min="13" style="0" width="31.9489795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="15.3010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1816,7 +1936,7 @@
       <c r="X27" s="5"/>
       <c r="Y27" s="5"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
         <v>40</v>
       </c>
@@ -1851,23 +1971,27 @@
       <c r="X28" s="5"/>
       <c r="Y28" s="5"/>
     </row>
-    <row r="29" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="41" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D29" s="5"/>
+      <c r="C29" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="E29" s="5"/>
-      <c r="F29" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
@@ -1886,21 +2010,21 @@
       <c r="X29" s="5"/>
       <c r="Y29" s="5"/>
     </row>
-    <row r="30" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>59</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" s="5"/>
       <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
+      <c r="F30" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
@@ -1922,22 +2046,14 @@
       <c r="Y30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>59</v>
-      </c>
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
@@ -1958,16 +2074,16 @@
     </row>
     <row r="32" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C32" s="5" t="s">
         <v>63</v>
       </c>
+      <c r="C32" s="7" t="s">
+        <v>64</v>
+      </c>
       <c r="D32" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
@@ -1991,9 +2107,9 @@
       <c r="X32" s="5"/>
       <c r="Y32" s="5"/>
     </row>
-    <row r="33" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>65</v>
@@ -2001,11 +2117,13 @@
       <c r="C33" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D33" s="5"/>
+      <c r="D33" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
@@ -2024,11 +2142,19 @@
       <c r="X33" s="5"/>
       <c r="Y33" s="5"/>
     </row>
-    <row r="34" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
+    <row r="34" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
@@ -2053,18 +2179,16 @@
     </row>
     <row r="35" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D35" s="5"/>
-      <c r="E35" s="8" t="s">
-        <v>69</v>
-      </c>
+      <c r="E35" s="5"/>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
@@ -2113,23 +2237,23 @@
       <c r="X36" s="5"/>
       <c r="Y36" s="5"/>
     </row>
-    <row r="37" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E37" s="5"/>
+        <v>73</v>
+      </c>
+      <c r="D37" s="5"/>
+      <c r="E37" s="8" t="s">
+        <v>74</v>
+      </c>
       <c r="F37" s="5"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
@@ -2149,22 +2273,14 @@
       <c r="Y37" s="5"/>
     </row>
     <row r="38" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>59</v>
-      </c>
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
       <c r="K38" s="5"/>
@@ -2185,7 +2301,7 @@
     </row>
     <row r="39" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>75</v>
@@ -2193,7 +2309,9 @@
       <c r="C39" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D39" s="5"/>
+      <c r="D39" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
       <c r="G39" s="4"/>
@@ -2217,10 +2335,18 @@
       <c r="Y39" s="5"/>
     </row>
     <row r="40" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
+      <c r="A40" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
       <c r="G40" s="4"/>
@@ -2244,14 +2370,20 @@
       <c r="Y40" s="5"/>
     </row>
     <row r="41" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
+      <c r="A41" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>80</v>
+      </c>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="5"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
       <c r="I41" s="5"/>
       <c r="J41" s="5"/>
       <c r="K41" s="5"/>
@@ -2271,16 +2403,14 @@
       <c r="Y41" s="5"/>
     </row>
     <row r="42" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
-      <c r="H42" s="5"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
       <c r="I42" s="5"/>
       <c r="J42" s="5"/>
       <c r="K42" s="5"/>
@@ -2300,7 +2430,7 @@
       <c r="Y42" s="5"/>
     </row>
     <row r="43" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="4"/>
+      <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
@@ -2327,7 +2457,9 @@
       <c r="Y43" s="5"/>
     </row>
     <row r="44" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="4"/>
+      <c r="A44" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
@@ -2356,7 +2488,7 @@
     <row r="45" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4"/>
       <c r="B45" s="5"/>
-      <c r="C45" s="7"/>
+      <c r="C45" s="5"/>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
@@ -2383,7 +2515,7 @@
     <row r="46" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="4"/>
       <c r="B46" s="5"/>
-      <c r="C46" s="7"/>
+      <c r="C46" s="5"/>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
@@ -2410,7 +2542,7 @@
     <row r="47" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="4"/>
       <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
+      <c r="C47" s="7"/>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
@@ -2436,61 +2568,61 @@
     </row>
     <row r="48" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="4"/>
-      <c r="B48" s="9"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
-      <c r="H48" s="4"/>
-      <c r="I48" s="4"/>
-      <c r="J48" s="4"/>
-      <c r="K48" s="4"/>
-      <c r="L48" s="4"/>
-      <c r="M48" s="4"/>
-      <c r="N48" s="4"/>
-      <c r="O48" s="4"/>
-      <c r="P48" s="4"/>
-      <c r="Q48" s="4"/>
-      <c r="R48" s="4"/>
-      <c r="S48" s="4"/>
-      <c r="T48" s="4"/>
-      <c r="U48" s="4"/>
-      <c r="V48" s="4"/>
-      <c r="W48" s="4"/>
-      <c r="X48" s="4"/>
-      <c r="Y48" s="4"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="5"/>
+      <c r="J48" s="5"/>
+      <c r="K48" s="5"/>
+      <c r="L48" s="5"/>
+      <c r="M48" s="5"/>
+      <c r="N48" s="5"/>
+      <c r="O48" s="5"/>
+      <c r="P48" s="5"/>
+      <c r="Q48" s="5"/>
+      <c r="R48" s="5"/>
+      <c r="S48" s="5"/>
+      <c r="T48" s="5"/>
+      <c r="U48" s="5"/>
+      <c r="V48" s="5"/>
+      <c r="W48" s="5"/>
+      <c r="X48" s="5"/>
+      <c r="Y48" s="5"/>
     </row>
     <row r="49" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="4"/>
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4"/>
-      <c r="G49" s="4"/>
-      <c r="H49" s="4"/>
-      <c r="I49" s="4"/>
-      <c r="J49" s="4"/>
-      <c r="K49" s="4"/>
-      <c r="L49" s="4"/>
-      <c r="M49" s="4"/>
-      <c r="N49" s="4"/>
-      <c r="O49" s="4"/>
-      <c r="P49" s="4"/>
-      <c r="Q49" s="4"/>
-      <c r="R49" s="4"/>
-      <c r="S49" s="4"/>
-      <c r="T49" s="4"/>
-      <c r="U49" s="4"/>
-      <c r="V49" s="4"/>
-      <c r="W49" s="4"/>
-      <c r="X49" s="4"/>
-      <c r="Y49" s="4"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="5"/>
+      <c r="J49" s="5"/>
+      <c r="K49" s="5"/>
+      <c r="L49" s="5"/>
+      <c r="M49" s="5"/>
+      <c r="N49" s="5"/>
+      <c r="O49" s="5"/>
+      <c r="P49" s="5"/>
+      <c r="Q49" s="5"/>
+      <c r="R49" s="5"/>
+      <c r="S49" s="5"/>
+      <c r="T49" s="5"/>
+      <c r="U49" s="5"/>
+      <c r="V49" s="5"/>
+      <c r="W49" s="5"/>
+      <c r="X49" s="5"/>
+      <c r="Y49" s="5"/>
     </row>
     <row r="50" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="4"/>
-      <c r="B50" s="4"/>
+      <c r="B50" s="9"/>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
@@ -2570,36 +2702,36 @@
       <c r="Y52" s="4"/>
     </row>
     <row r="53" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="5"/>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5"/>
-      <c r="F53" s="5"/>
-      <c r="G53" s="5"/>
-      <c r="H53" s="5"/>
-      <c r="I53" s="5"/>
-      <c r="J53" s="5"/>
-      <c r="K53" s="5"/>
-      <c r="L53" s="5"/>
-      <c r="M53" s="5"/>
-      <c r="N53" s="5"/>
-      <c r="O53" s="5"/>
-      <c r="P53" s="5"/>
-      <c r="Q53" s="5"/>
-      <c r="R53" s="5"/>
-      <c r="S53" s="5"/>
-      <c r="T53" s="5"/>
-      <c r="U53" s="5"/>
-      <c r="V53" s="5"/>
-      <c r="W53" s="5"/>
-      <c r="X53" s="5"/>
-      <c r="Y53" s="5"/>
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4"/>
+      <c r="K53" s="4"/>
+      <c r="L53" s="4"/>
+      <c r="M53" s="4"/>
+      <c r="N53" s="4"/>
+      <c r="O53" s="4"/>
+      <c r="P53" s="4"/>
+      <c r="Q53" s="4"/>
+      <c r="R53" s="4"/>
+      <c r="S53" s="4"/>
+      <c r="T53" s="4"/>
+      <c r="U53" s="4"/>
+      <c r="V53" s="4"/>
+      <c r="W53" s="4"/>
+      <c r="X53" s="4"/>
+      <c r="Y53" s="4"/>
     </row>
     <row r="54" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
-      <c r="C54" s="7"/>
+      <c r="C54" s="4"/>
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
@@ -2624,12 +2756,12 @@
       <c r="Y54" s="4"/>
     </row>
     <row r="55" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="4"/>
+      <c r="A55" s="5"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
-      <c r="E55" s="4"/>
-      <c r="F55" s="4"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
       <c r="G55" s="5"/>
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
@@ -2652,38 +2784,38 @@
     </row>
     <row r="56" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="4"/>
-      <c r="B56" s="5"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="5"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="4"/>
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
-      <c r="G56" s="5"/>
-      <c r="H56" s="5"/>
-      <c r="I56" s="5"/>
-      <c r="J56" s="5"/>
-      <c r="K56" s="5"/>
-      <c r="L56" s="5"/>
-      <c r="M56" s="5"/>
-      <c r="N56" s="5"/>
-      <c r="O56" s="5"/>
-      <c r="P56" s="5"/>
-      <c r="Q56" s="5"/>
-      <c r="R56" s="5"/>
-      <c r="S56" s="5"/>
-      <c r="T56" s="5"/>
-      <c r="U56" s="5"/>
-      <c r="V56" s="5"/>
-      <c r="W56" s="5"/>
-      <c r="X56" s="5"/>
-      <c r="Y56" s="5"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="4"/>
+      <c r="J56" s="4"/>
+      <c r="K56" s="4"/>
+      <c r="L56" s="4"/>
+      <c r="M56" s="4"/>
+      <c r="N56" s="4"/>
+      <c r="O56" s="4"/>
+      <c r="P56" s="4"/>
+      <c r="Q56" s="4"/>
+      <c r="R56" s="4"/>
+      <c r="S56" s="4"/>
+      <c r="T56" s="4"/>
+      <c r="U56" s="4"/>
+      <c r="V56" s="4"/>
+      <c r="W56" s="4"/>
+      <c r="X56" s="4"/>
+      <c r="Y56" s="4"/>
     </row>
     <row r="57" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="5"/>
+      <c r="A57" s="4"/>
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
-      <c r="E57" s="5"/>
-      <c r="F57" s="5"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
       <c r="G57" s="5"/>
       <c r="H57" s="5"/>
       <c r="I57" s="5"/>
@@ -2706,38 +2838,38 @@
     </row>
     <row r="58" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="4"/>
-      <c r="B58" s="4"/>
-      <c r="C58" s="4"/>
-      <c r="D58" s="4"/>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
-      <c r="G58" s="4"/>
-      <c r="H58" s="4"/>
-      <c r="I58" s="4"/>
-      <c r="J58" s="4"/>
-      <c r="K58" s="4"/>
-      <c r="L58" s="4"/>
-      <c r="M58" s="4"/>
-      <c r="N58" s="4"/>
-      <c r="O58" s="4"/>
-      <c r="P58" s="4"/>
-      <c r="Q58" s="4"/>
-      <c r="R58" s="4"/>
-      <c r="S58" s="4"/>
-      <c r="T58" s="4"/>
-      <c r="U58" s="4"/>
-      <c r="V58" s="4"/>
-      <c r="W58" s="4"/>
-      <c r="X58" s="4"/>
-      <c r="Y58" s="4"/>
+      <c r="G58" s="5"/>
+      <c r="H58" s="5"/>
+      <c r="I58" s="5"/>
+      <c r="J58" s="5"/>
+      <c r="K58" s="5"/>
+      <c r="L58" s="5"/>
+      <c r="M58" s="5"/>
+      <c r="N58" s="5"/>
+      <c r="O58" s="5"/>
+      <c r="P58" s="5"/>
+      <c r="Q58" s="5"/>
+      <c r="R58" s="5"/>
+      <c r="S58" s="5"/>
+      <c r="T58" s="5"/>
+      <c r="U58" s="5"/>
+      <c r="V58" s="5"/>
+      <c r="W58" s="5"/>
+      <c r="X58" s="5"/>
+      <c r="Y58" s="5"/>
     </row>
     <row r="59" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="4"/>
+      <c r="A59" s="5"/>
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
-      <c r="E59" s="4"/>
-      <c r="F59" s="4"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
       <c r="G59" s="5"/>
       <c r="H59" s="5"/>
       <c r="I59" s="5"/>
@@ -2786,12 +2918,12 @@
       <c r="Y60" s="4"/>
     </row>
     <row r="61" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="5"/>
+      <c r="A61" s="4"/>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
-      <c r="E61" s="5"/>
-      <c r="F61" s="5"/>
+      <c r="E61" s="4"/>
+      <c r="F61" s="4"/>
       <c r="G61" s="5"/>
       <c r="H61" s="5"/>
       <c r="I61" s="5"/>
@@ -2813,64 +2945,64 @@
       <c r="Y61" s="5"/>
     </row>
     <row r="62" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="10"/>
+      <c r="A62" s="4"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
-      <c r="G62" s="11"/>
-      <c r="H62" s="11"/>
-      <c r="I62" s="11"/>
-      <c r="J62" s="11"/>
-      <c r="K62" s="11"/>
-      <c r="L62" s="11"/>
-      <c r="M62" s="11"/>
-      <c r="N62" s="11"/>
-      <c r="O62" s="11"/>
-      <c r="P62" s="11"/>
-      <c r="Q62" s="11"/>
-      <c r="R62" s="11"/>
-      <c r="S62" s="11"/>
-      <c r="T62" s="11"/>
-      <c r="U62" s="11"/>
-      <c r="V62" s="11"/>
-      <c r="W62" s="11"/>
-      <c r="X62" s="11"/>
-      <c r="Y62" s="11"/>
+      <c r="G62" s="4"/>
+      <c r="H62" s="4"/>
+      <c r="I62" s="4"/>
+      <c r="J62" s="4"/>
+      <c r="K62" s="4"/>
+      <c r="L62" s="4"/>
+      <c r="M62" s="4"/>
+      <c r="N62" s="4"/>
+      <c r="O62" s="4"/>
+      <c r="P62" s="4"/>
+      <c r="Q62" s="4"/>
+      <c r="R62" s="4"/>
+      <c r="S62" s="4"/>
+      <c r="T62" s="4"/>
+      <c r="U62" s="4"/>
+      <c r="V62" s="4"/>
+      <c r="W62" s="4"/>
+      <c r="X62" s="4"/>
+      <c r="Y62" s="4"/>
     </row>
     <row r="63" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="10"/>
-      <c r="B63" s="4"/>
-      <c r="C63" s="4"/>
-      <c r="D63" s="11"/>
-      <c r="E63" s="4"/>
-      <c r="F63" s="4"/>
-      <c r="G63" s="11"/>
-      <c r="H63" s="11"/>
-      <c r="I63" s="11"/>
-      <c r="J63" s="11"/>
-      <c r="K63" s="11"/>
-      <c r="L63" s="11"/>
-      <c r="M63" s="11"/>
-      <c r="N63" s="11"/>
-      <c r="O63" s="11"/>
-      <c r="P63" s="11"/>
-      <c r="Q63" s="11"/>
-      <c r="R63" s="11"/>
-      <c r="S63" s="11"/>
-      <c r="T63" s="11"/>
-      <c r="U63" s="11"/>
-      <c r="V63" s="11"/>
-      <c r="W63" s="11"/>
-      <c r="X63" s="11"/>
-      <c r="Y63" s="11"/>
+      <c r="A63" s="5"/>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="5"/>
+      <c r="G63" s="5"/>
+      <c r="H63" s="5"/>
+      <c r="I63" s="5"/>
+      <c r="J63" s="5"/>
+      <c r="K63" s="5"/>
+      <c r="L63" s="5"/>
+      <c r="M63" s="5"/>
+      <c r="N63" s="5"/>
+      <c r="O63" s="5"/>
+      <c r="P63" s="5"/>
+      <c r="Q63" s="5"/>
+      <c r="R63" s="5"/>
+      <c r="S63" s="5"/>
+      <c r="T63" s="5"/>
+      <c r="U63" s="5"/>
+      <c r="V63" s="5"/>
+      <c r="W63" s="5"/>
+      <c r="X63" s="5"/>
+      <c r="Y63" s="5"/>
     </row>
     <row r="64" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="10"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
-      <c r="D64" s="11"/>
+      <c r="D64" s="4"/>
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
       <c r="G64" s="11"/>
@@ -2893,132 +3025,185 @@
       <c r="X64" s="11"/>
       <c r="Y64" s="11"/>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="65" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="10"/>
+      <c r="B65" s="4"/>
+      <c r="C65" s="4"/>
+      <c r="D65" s="11"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="4"/>
+      <c r="G65" s="11"/>
+      <c r="H65" s="11"/>
+      <c r="I65" s="11"/>
+      <c r="J65" s="11"/>
+      <c r="K65" s="11"/>
+      <c r="L65" s="11"/>
+      <c r="M65" s="11"/>
+      <c r="N65" s="11"/>
+      <c r="O65" s="11"/>
+      <c r="P65" s="11"/>
+      <c r="Q65" s="11"/>
+      <c r="R65" s="11"/>
+      <c r="S65" s="11"/>
+      <c r="T65" s="11"/>
+      <c r="U65" s="11"/>
+      <c r="V65" s="11"/>
+      <c r="W65" s="11"/>
+      <c r="X65" s="11"/>
+      <c r="Y65" s="11"/>
+    </row>
+    <row r="66" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="10"/>
+      <c r="B66" s="4"/>
+      <c r="C66" s="4"/>
+      <c r="D66" s="11"/>
+      <c r="E66" s="4"/>
+      <c r="F66" s="4"/>
+      <c r="G66" s="11"/>
+      <c r="H66" s="11"/>
+      <c r="I66" s="11"/>
+      <c r="J66" s="11"/>
+      <c r="K66" s="11"/>
+      <c r="L66" s="11"/>
+      <c r="M66" s="11"/>
+      <c r="N66" s="11"/>
+      <c r="O66" s="11"/>
+      <c r="P66" s="11"/>
+      <c r="Q66" s="11"/>
+      <c r="R66" s="11"/>
+      <c r="S66" s="11"/>
+      <c r="T66" s="11"/>
+      <c r="U66" s="11"/>
+      <c r="V66" s="11"/>
+      <c r="W66" s="11"/>
+      <c r="X66" s="11"/>
+      <c r="Y66" s="11"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:Y26,A29:Y1020">
-    <cfRule type="containsText" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:Y26,A29:Y1005">
-    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>AND($A1="begin group", NOT($B1 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:Y26,A29:Y1020">
-    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>AND($A1="end group", $B1 = "", $C1 = "", $D1 = "", $E1 = "", $F1 = "", $G1 = "", $H1 = "", $I1 = "", $J1 = "", $K1 = "", $L1 = "", $M1 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:Y26,A29:Y1020">
-    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
-      <formula>"note"</formula>
+  <conditionalFormatting sqref="A1">
+    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>AND(A1 = "type", COUNTIF($A$1:$A$1016, "begin group") = COUNTIF($A$1:$A$1016, "end group"))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>AND(A1 = "type", COUNTIF($A$1:$A$1014, "begin group") = COUNTIF($A$1:$A$1014, "end group"))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1">
-    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
-      <formula>OR(NOT(A1 = "type"), NOT(COUNTIF($A$1:$A$1005, "begin group") = COUNTIF($A$1:$A$1014, "end group")))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I1:I26,I29:I1020">
-    <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
-      <formula>AND($I1 = "", $A1 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C26,C29:C1020">
-    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
-      <formula>AND(AND(NOT($A1 = "end group"), NOT($A1 = "end repeat"), NOT($A1 = "")), $C1 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B26,B29:B1020">
-    <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
-      <formula>AND(AND(NOT($A1 = "end group"), NOT($A1 = "end repeat"), NOT($A1 = "")), $B1 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A26,A29:A1020">
-    <cfRule type="cellIs" priority="11" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
-      <formula>"hidden"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B26,B29:B1013">
-    <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
-      <formula>COUNTIF($B$2:$B$1013,B2)&gt;1</formula>
+    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>OR(NOT(A1 = "type"), NOT(COUNTIF($A$1:$A$1007, "begin group") = COUNTIF($A$1:$A$1016, "end group")))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1">
-    <cfRule type="cellIs" priority="13" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="cellIs" priority="4" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>"name"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1">
-    <cfRule type="notContainsText" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="label" dxfId="12"/>
+    <cfRule type="notContainsText" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="label" dxfId="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1">
-    <cfRule type="cellIs" priority="15" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
+    <cfRule type="cellIs" priority="6" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
       <formula>"required"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1">
-    <cfRule type="cellIs" priority="16" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
+    <cfRule type="cellIs" priority="7" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
       <formula>"relevant"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="cellIs" priority="17" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
+    <cfRule type="cellIs" priority="8" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
       <formula>"appearance"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1">
-    <cfRule type="cellIs" priority="18" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
+    <cfRule type="cellIs" priority="9" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
       <formula>"constraint"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="notContainsText" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="constraint_message" dxfId="17"/>
+    <cfRule type="notContainsText" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="constraint_message" dxfId="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1">
-    <cfRule type="cellIs" priority="20" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18">
+    <cfRule type="cellIs" priority="11" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18">
       <formula>"calculation"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1">
-    <cfRule type="cellIs" priority="21" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19">
+    <cfRule type="cellIs" priority="12" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19">
       <formula>"choice_filter"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1">
-    <cfRule type="notContainsText" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="hint" dxfId="20"/>
+    <cfRule type="notContainsText" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="hint" dxfId="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1">
-    <cfRule type="cellIs" priority="23" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21">
+    <cfRule type="cellIs" priority="14" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21">
       <formula>"default"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:Y1">
-    <cfRule type="cellIs" priority="24" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22">
+    <cfRule type="cellIs" priority="15" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22">
       <formula>"media::image"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H26,H29:H1005">
-    <cfRule type="expression" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23">
-      <formula>AND(NOT($G1 = ""), $H1 = "")</formula>
+  <conditionalFormatting sqref="A29:Y29">
+    <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26">
+      <formula>AND($A29="begin group", NOT($B29 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:Y26,A29:Y1005">
-    <cfRule type="expression" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24">
-      <formula>AND($A1="begin repeat", NOT($B1 = ""))</formula>
+  <conditionalFormatting sqref="A29:Y29">
+    <cfRule type="expression" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27">
+      <formula>AND($A29="end group", $B29 = "", $C29 = "", $D29 = "", $E29 = "", $F29 = "", $G29 = "", $H29 = "", $I29 = "", $J29 = "", $K29 = "", $L29 = "", $M29 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:Y26,A29:Y1020">
-    <cfRule type="expression" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25">
-      <formula>AND($A1="end repeat", $B1 = "", $C1 = "", $D1 = "", $E1 = "", $F1 = "", $G1 = "", $H1 = "", $I1 = "", $J1 = "", $K1 = "", $L1 = "", $M1 = "")</formula>
+  <conditionalFormatting sqref="A29:Y29">
+    <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
+      <formula>AND($A29="begin repeat", NOT($B29 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A29:Y29">
+    <cfRule type="expression" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29">
+      <formula>AND($A29="end repeat", $B29 = "", $C29 = "", $D29 = "", $E29 = "", $F29 = "", $G29 = "", $H29 = "", $I29 = "", $J29 = "", $K29 = "", $L29 = "", $M29 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I29">
+    <cfRule type="expression" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30">
+      <formula>AND($I29 = "", $A29 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C29">
+    <cfRule type="expression" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31">
+      <formula>AND(AND(NOT($A29 = "end group"), NOT($A29 = "end repeat"), NOT($A29 = "")), $C29 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B29">
+    <cfRule type="expression" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32">
+      <formula>AND(AND(NOT($A29 = "end group"), NOT($A29 = "end repeat"), NOT($A29 = "")), $B29 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H29">
+    <cfRule type="expression" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33">
+      <formula>AND(NOT($G29 = ""), $H29 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B29">
+    <cfRule type="expression" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34">
+      <formula>COUNTIF($B$2:$B$1048,B29)&gt;1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A29:Y29">
+    <cfRule type="containsText" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="35"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A29:Y29">
+    <cfRule type="cellIs" priority="26" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="36">
+      <formula>"note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A29">
+    <cfRule type="cellIs" priority="27" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="37">
+      <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D2:D64" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D2:D66" type="list">
       <formula1>"yes,no"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3048,15 +3233,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.219387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.5"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.3571428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.2959183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.8469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="15.3010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>1</v>
@@ -3070,13 +3255,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D2" s="14"/>
       <c r="E2" s="14"/>
@@ -3084,13 +3269,13 @@
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
@@ -3106,13 +3291,13 @@
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="14"/>
@@ -3120,13 +3305,13 @@
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="14" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
@@ -3134,13 +3319,13 @@
     </row>
     <row r="7" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="14" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
@@ -3148,13 +3333,13 @@
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="14" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
@@ -3162,13 +3347,13 @@
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="14" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
@@ -3201,47 +3386,47 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="15.3010204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="15.3010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C2" s="15" t="n">
         <f aca="true">NOW()</f>
-        <v>44056.7421792928</v>
+        <v>44060.4977124069</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="F2" s="14"/>
     </row>

</xml_diff>

<commit_message>
cleaned up hts forms. cleaned up the workflow
</commit_message>
<xml_diff>
--- a/config/default/forms/app/hts_linkage.xlsx
+++ b/config/default/forms/app/hts_linkage.xlsx
@@ -1,19 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grmfutures-my.sharepoint.com/personal/valentine_komulo_thepalladiumgroup_com/Documents/eHTS_Forms/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{A14EC8C9-1521-491F-841E-0FDEDD1C7AAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{541FCC60-3FDC-42BF-8A3F-8F0B73BFE9A5}"/>
+  <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="996" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13096" tabRatio="994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="choices" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="settings" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="survey" sheetId="1" r:id="rId1"/>
+    <sheet name="choices" sheetId="2" r:id="rId2"/>
+    <sheet name="settings" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
@@ -22,341 +36,358 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="108">
-  <si>
-    <t xml:space="preserve">type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">label</t>
-  </si>
-  <si>
-    <t xml:space="preserve">required</t>
-  </si>
-  <si>
-    <t xml:space="preserve">relevant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">appearance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">constraint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">constraint_message::en</t>
-  </si>
-  <si>
-    <t xml:space="preserve">calculation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">choice_filter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">default</t>
-  </si>
-  <si>
-    <t xml:space="preserve">media::image</t>
-  </si>
-  <si>
-    <t xml:space="preserve">begin group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inputs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Patient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./source = 'user'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">field-list</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hidden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">source</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Source</t>
-  </si>
-  <si>
-    <t xml:space="preserve">user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">source_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Source ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contact</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact</t>
-  </si>
-  <si>
-    <t xml:space="preserve">db:clinic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What is the patient's name?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">db-object</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">db:person</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID of head of household</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name of head of household</t>
-  </si>
-  <si>
-    <t xml:space="preserve">end group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">parent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHW name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHW phone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">calculate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NO_LABEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../inputs/source</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../inputs/source_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">place_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../inputs/contact/_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">place_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../inputs/contact/name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">head</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../inputs/contact/contact/name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">form_uuid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">'050a7f12-5c52-4cad-8834-863695af335d'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">encounter_type_uuid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">'9c0a7a57-62ff-4f75-babe-5835b0e921b7'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">encounter_date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date of linkage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">floor(decimal-date-time(.)) &lt;= floor(decimal-date-time(today())) and floor( difference-in-months( . , today() ) div 12 ) &lt;= 100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Encounter date can not be in the future</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hts_linkage_assessment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Linkage to care</t>
-  </si>
-  <si>
-    <t xml:space="preserve">text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_162724_facilityLinkedTo_99DCT</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="114">
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>relevant</t>
+  </si>
+  <si>
+    <t>appearance</t>
+  </si>
+  <si>
+    <t>constraint</t>
+  </si>
+  <si>
+    <t>constraint_message::en</t>
+  </si>
+  <si>
+    <t>calculation</t>
+  </si>
+  <si>
+    <t>choice_filter</t>
+  </si>
+  <si>
+    <t>hint</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>media::image</t>
+  </si>
+  <si>
+    <t>begin group</t>
+  </si>
+  <si>
+    <t>inputs</t>
+  </si>
+  <si>
+    <t>Patient</t>
+  </si>
+  <si>
+    <t>./source = 'user'</t>
+  </si>
+  <si>
+    <t>field-list</t>
+  </si>
+  <si>
+    <t>hidden</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>source_id</t>
+  </si>
+  <si>
+    <t>Source ID</t>
+  </si>
+  <si>
+    <t>contact</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>db:clinic</t>
+  </si>
+  <si>
+    <t>_id</t>
+  </si>
+  <si>
+    <t>What is the patient's name?</t>
+  </si>
+  <si>
+    <t>db-object</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>db:person</t>
+  </si>
+  <si>
+    <t>ID of head of household</t>
+  </si>
+  <si>
+    <t>Name of head of household</t>
+  </si>
+  <si>
+    <t>end group</t>
+  </si>
+  <si>
+    <t>parent</t>
+  </si>
+  <si>
+    <t>Parent</t>
+  </si>
+  <si>
+    <t>CHW name</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>CHW phone</t>
+  </si>
+  <si>
+    <t>calculate</t>
+  </si>
+  <si>
+    <t>NO_LABEL</t>
+  </si>
+  <si>
+    <t>../inputs/source</t>
+  </si>
+  <si>
+    <t>../inputs/source_id</t>
+  </si>
+  <si>
+    <t>place_id</t>
+  </si>
+  <si>
+    <t>../inputs/contact/_id</t>
+  </si>
+  <si>
+    <t>place_name</t>
+  </si>
+  <si>
+    <t>../inputs/contact/name</t>
+  </si>
+  <si>
+    <t>head</t>
+  </si>
+  <si>
+    <t>../inputs/contact/contact/name</t>
+  </si>
+  <si>
+    <t>form_uuid</t>
+  </si>
+  <si>
+    <t>'050a7f12-5c52-4cad-8834-863695af335d'</t>
+  </si>
+  <si>
+    <t>encounter_type_uuid</t>
+  </si>
+  <si>
+    <t>'9c0a7a57-62ff-4f75-babe-5835b0e921b7'</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>encounter_date</t>
+  </si>
+  <si>
+    <t>Date of linkage</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>floor(decimal-date-time(.)) &lt;= floor(decimal-date-time(today())) and floor( difference-in-months( . , today() ) div 12 ) &lt;= 100</t>
+  </si>
+  <si>
+    <t>Encounter date cannot be in the future</t>
+  </si>
+  <si>
+    <t>hts_linkage_assessment</t>
+  </si>
+  <si>
+    <t>Linkage to care</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>_162724_facilityLinkedTo_99DCT</t>
   </si>
   <si>
     <t xml:space="preserve">Facility linked to:  </t>
   </si>
   <si>
-    <t xml:space="preserve">_162053_cccNumber_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCC number:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_1473_healthWorkerHandedTo_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Health worker handed to</t>
-  </si>
-  <si>
-    <t xml:space="preserve">select_one cadre_of_health_worker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_162577_cadreOfHealthWorker_99DCT</t>
+    <t>_162053_cccNumber_99DCT</t>
+  </si>
+  <si>
+    <t>CCC number:</t>
+  </si>
+  <si>
+    <t>regex(.,'^[0-9]{10}$')</t>
+  </si>
+  <si>
+    <t>CCC Number should be 10 digits</t>
+  </si>
+  <si>
+    <t>_1473_healthWorkerHandedTo_99DCT</t>
+  </si>
+  <si>
+    <t>Health worker handed to</t>
+  </si>
+  <si>
+    <t>select_one cadre_of_health_worker</t>
+  </si>
+  <si>
+    <t>_162577_cadreOfHealthWorker_99DCT</t>
   </si>
   <si>
     <t xml:space="preserve">Cadre of health worker : </t>
   </si>
   <si>
-    <t xml:space="preserve">_164401_otherCadre_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Specify other cadre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${_162577_cadreOfHealthWorker_99DCT}=”_5622_other_99DCT”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_160555_dateEnrolled_99DCT</t>
+    <t>_164401_otherCadre_99DCT</t>
+  </si>
+  <si>
+    <t>Specify other cadre</t>
+  </si>
+  <si>
+    <t>${_162577_cadreOfHealthWorker_99DCT}=”_5622_other_99DCT”</t>
+  </si>
+  <si>
+    <t>_160555_dateEnrolled_99DCT</t>
   </si>
   <si>
     <t xml:space="preserve">Date enrolled : </t>
   </si>
   <si>
-    <t xml:space="preserve">_159599_ARTdate_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ART start date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_163042_remarks_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Remark(s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">list_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes_no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_1065_yes_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_1066_no_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cadre_of_health_worker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_1577_nurse_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nurse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_1574_clinicalOficer_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clincal officer/Docter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_1555_communityHealthWorker_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Community health care worker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_1540_employess_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Employee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_5622_other_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other</t>
-  </si>
-  <si>
-    <t xml:space="preserve">form_title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">form_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">version</t>
-  </si>
-  <si>
-    <t xml:space="preserve">style</t>
-  </si>
-  <si>
-    <t xml:space="preserve">path</t>
-  </si>
-  <si>
-    <t xml:space="preserve">instance_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HTS Linkage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hts_linkage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pages</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data</t>
+    <t>. &gt;= ${encounter_date} and . &lt;= today()</t>
+  </si>
+  <si>
+    <t>_159599_ARTdate_99DCT</t>
+  </si>
+  <si>
+    <t>ART start date</t>
+  </si>
+  <si>
+    <t>. &gt;= ${_160555_dateEnrolled_99DCT} and . &lt;= today()</t>
+  </si>
+  <si>
+    <t>_163042_remarks_99DCT</t>
+  </si>
+  <si>
+    <t>Remark(s)</t>
+  </si>
+  <si>
+    <t>list_name</t>
+  </si>
+  <si>
+    <t>yes_no</t>
+  </si>
+  <si>
+    <t>_1065_yes_99DCT</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>_1066_no_99DCT</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>cadre_of_health_worker</t>
+  </si>
+  <si>
+    <t>_1577_nurse_99DCT</t>
+  </si>
+  <si>
+    <t>Nurse</t>
+  </si>
+  <si>
+    <t>_1574_clinicalOficer_99DCT</t>
+  </si>
+  <si>
+    <t>Clincal officer/Docter</t>
+  </si>
+  <si>
+    <t>_1555_communityHealthWorker_99DCT</t>
+  </si>
+  <si>
+    <t>Community health care worker</t>
+  </si>
+  <si>
+    <t>_1540_employess_99DCT</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>_5622_other_99DCT</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>form_title</t>
+  </si>
+  <si>
+    <t>form_id</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>style</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>instance_name</t>
+  </si>
+  <si>
+    <t>HTS Linkage</t>
+  </si>
+  <si>
+    <t>hts_linkage</t>
+  </si>
+  <si>
+    <t>pages</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>ART start date cannot be before enrollment date and can not also be in the future</t>
+  </si>
+  <si>
+    <t>Date enrolled cannot be in the future or HIV test date.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD\-MM\-YYYY\ HH\-MM\-SS"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy\ hh\-mm\-ss"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -365,22 +396,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -410,9 +426,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF4C4C4C"/>
       <name val="Ubuntu"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -456,7 +483,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -464,133 +491,72 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="18">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="16">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="38">
+  <dxfs count="28">
     <dxf>
       <font>
-        <color rgb="FFB7B7B7"/>
+        <color rgb="FFCCCCCC"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF76A5AF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCFE2F3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC27BA0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCFE2F3"/>
+          <bgColor rgb="FFFFF2CC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -605,54 +571,12 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
-        <strike val="1"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFB7B7B7"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF980000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFCCCCCC"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFD9EAD3"/>
         </patternFill>
       </fill>
     </dxf>
@@ -660,215 +584,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFEAD1DC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="1"/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="1"/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="1"/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="1"/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="1"/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="1"/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="1"/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="1"/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="1"/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="1"/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="1"/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="1"/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF76A5AF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9D2E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC27BA0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9D2E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF76A5AF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCFE2F3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC27BA0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCFE2F3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF76A5AF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9D2E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC27BA0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9D2E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF980000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -894,43 +609,234 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFEAD1DC"/>
+          <bgColor rgb="FF980000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFB7B7B7"/>
+        <color rgb="FFC27BA0"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9D2E9"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFCCCCCC"/>
+        <color rgb="FF76A5AF"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFD9D2E9"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFCCCCCC"/>
+        <color rgb="FFC27BA0"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFCFE2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF76A5AF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCFE2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
     </dxf>
   </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{730D7CB3-FC78-4401-868C-4768F9C589F6}">
+      <tableStyleElement type="wholeTable" dxfId="27"/>
+      <tableStyleElement type="headerRow" dxfId="26"/>
+    </tableStyle>
+  </tableStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -989,45 +895,352 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF4C4C4C"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y66"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I28" activeCellId="0" sqref="I28"/>
+    <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+      <selection pane="bottomRight" activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.1479591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.3265306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.015306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.3010204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="56.2448979591837"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.5408163265306"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.3979591836735"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="35.0102040816326"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="79.1938775510204"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.3010204081633"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="26.8163265306122"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.3010204081633"/>
-    <col collapsed="false" hidden="false" max="25" min="13" style="0" width="31.9489795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="15.3010204081633"/>
+    <col min="1" max="1" width="30.1328125"/>
+    <col min="2" max="2" width="30.265625"/>
+    <col min="3" max="3" width="35.3984375"/>
+    <col min="4" max="4" width="0" hidden="1"/>
+    <col min="5" max="5" width="4.3984375"/>
+    <col min="6" max="6" width="18.59765625"/>
+    <col min="7" max="7" width="41.3984375"/>
+    <col min="8" max="8" width="66.73046875"/>
+    <col min="9" max="9" width="79.1328125"/>
+    <col min="10" max="10" width="15.265625"/>
+    <col min="11" max="11" width="26.86328125"/>
+    <col min="12" max="12" width="15.265625"/>
+    <col min="13" max="25" width="32"/>
+    <col min="26" max="1025" width="15.265625"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:25" ht="41.65">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1080,7 +1293,7 @@
       <c r="X1" s="2"/>
       <c r="Y1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:25" ht="67.5">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -1117,7 +1330,7 @@
       <c r="X2" s="4"/>
       <c r="Y2" s="4"/>
     </row>
-    <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:25" ht="13.5">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -1152,7 +1365,7 @@
       <c r="X3" s="4"/>
       <c r="Y3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:25" ht="13.5">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
@@ -1185,7 +1398,7 @@
       <c r="X4" s="4"/>
       <c r="Y4" s="4"/>
     </row>
-    <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:25" ht="13.5">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -1218,7 +1431,7 @@
       <c r="X5" s="4"/>
       <c r="Y5" s="4"/>
     </row>
-    <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:25" ht="13.5">
       <c r="A6" s="3" t="s">
         <v>26</v>
       </c>
@@ -1253,7 +1466,7 @@
       <c r="X6" s="4"/>
       <c r="Y6" s="4"/>
     </row>
-    <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:25" ht="13.5">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -1286,7 +1499,7 @@
       <c r="X7" s="4"/>
       <c r="Y7" s="4"/>
     </row>
-    <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:25" ht="13.5">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
@@ -1319,7 +1532,7 @@
       <c r="X8" s="4"/>
       <c r="Y8" s="4"/>
     </row>
-    <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:25" ht="13.5">
       <c r="A9" s="3" t="s">
         <v>31</v>
       </c>
@@ -1354,7 +1567,7 @@
       <c r="X9" s="4"/>
       <c r="Y9" s="4"/>
     </row>
-    <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:25" ht="13.5">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
@@ -1387,7 +1600,7 @@
       <c r="X10" s="4"/>
       <c r="Y10" s="4"/>
     </row>
-    <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:25" ht="13.5">
       <c r="A11" s="3" t="s">
         <v>34</v>
       </c>
@@ -1416,7 +1629,7 @@
       <c r="X11" s="4"/>
       <c r="Y11" s="4"/>
     </row>
-    <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:25" ht="13.5">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
@@ -1449,7 +1662,7 @@
       <c r="X12" s="4"/>
       <c r="Y12" s="4"/>
     </row>
-    <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:25" ht="13.5">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
@@ -1482,7 +1695,7 @@
       <c r="X13" s="4"/>
       <c r="Y13" s="4"/>
     </row>
-    <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:25" ht="13.5">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -1515,7 +1728,7 @@
       <c r="X14" s="4"/>
       <c r="Y14" s="4"/>
     </row>
-    <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:25" ht="13.5">
       <c r="A15" s="3" t="s">
         <v>18</v>
       </c>
@@ -1548,7 +1761,7 @@
       <c r="X15" s="4"/>
       <c r="Y15" s="4"/>
     </row>
-    <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:25" ht="13.5">
       <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
@@ -1581,7 +1794,7 @@
       <c r="X16" s="4"/>
       <c r="Y16" s="4"/>
     </row>
-    <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:25" ht="13.5">
       <c r="A17" s="3" t="s">
         <v>34</v>
       </c>
@@ -1610,7 +1823,7 @@
       <c r="X17" s="4"/>
       <c r="Y17" s="4"/>
     </row>
-    <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:25" ht="13.5">
       <c r="A18" s="3" t="s">
         <v>34</v>
       </c>
@@ -1639,7 +1852,7 @@
       <c r="X18" s="4"/>
       <c r="Y18" s="4"/>
     </row>
-    <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:25" ht="13.5">
       <c r="A19" s="3" t="s">
         <v>34</v>
       </c>
@@ -1668,7 +1881,7 @@
       <c r="X19" s="4"/>
       <c r="Y19" s="4"/>
     </row>
-    <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:25" ht="13.5">
       <c r="A20" s="3" t="s">
         <v>34</v>
       </c>
@@ -1697,7 +1910,7 @@
       <c r="X20" s="4"/>
       <c r="Y20" s="4"/>
     </row>
-    <row r="21" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:25" ht="13.5">
       <c r="A21" s="3" t="s">
         <v>34</v>
       </c>
@@ -1726,7 +1939,7 @@
       <c r="X21" s="4"/>
       <c r="Y21" s="4"/>
     </row>
-    <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:25" ht="13.5">
       <c r="A22" s="3" t="s">
         <v>40</v>
       </c>
@@ -1761,7 +1974,7 @@
       <c r="X22" s="4"/>
       <c r="Y22" s="4"/>
     </row>
-    <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:25" ht="13.5">
       <c r="A23" s="3" t="s">
         <v>40</v>
       </c>
@@ -1796,7 +2009,7 @@
       <c r="X23" s="4"/>
       <c r="Y23" s="4"/>
     </row>
-    <row r="24" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:25" ht="13.5">
       <c r="A24" s="5" t="s">
         <v>40</v>
       </c>
@@ -1831,7 +2044,7 @@
       <c r="X24" s="5"/>
       <c r="Y24" s="5"/>
     </row>
-    <row r="25" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:25" ht="13.5">
       <c r="A25" s="5" t="s">
         <v>40</v>
       </c>
@@ -1866,7 +2079,7 @@
       <c r="X25" s="5"/>
       <c r="Y25" s="5"/>
     </row>
-    <row r="26" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:25" ht="13.5">
       <c r="A26" s="5" t="s">
         <v>40</v>
       </c>
@@ -1901,7 +2114,7 @@
       <c r="X26" s="5"/>
       <c r="Y26" s="5"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:25" ht="13.5">
       <c r="A27" s="5" t="s">
         <v>40</v>
       </c>
@@ -1936,7 +2149,7 @@
       <c r="X27" s="5"/>
       <c r="Y27" s="5"/>
     </row>
-    <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:25" ht="13.5">
       <c r="A28" s="5" t="s">
         <v>40</v>
       </c>
@@ -1971,7 +2184,7 @@
       <c r="X28" s="5"/>
       <c r="Y28" s="5"/>
     </row>
-    <row r="29" customFormat="false" ht="41" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:25" ht="40.5">
       <c r="A29" s="5" t="s">
         <v>54</v>
       </c>
@@ -2010,7 +2223,7 @@
       <c r="X29" s="5"/>
       <c r="Y29" s="5"/>
     </row>
-    <row r="30" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:25" ht="14.25">
       <c r="A30" s="5" t="s">
         <v>13</v>
       </c>
@@ -2045,7 +2258,7 @@
       <c r="X30" s="5"/>
       <c r="Y30" s="5"/>
     </row>
-    <row r="31" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:25" ht="13.5">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="7"/>
@@ -2072,7 +2285,7 @@
       <c r="X31" s="5"/>
       <c r="Y31" s="5"/>
     </row>
-    <row r="32" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:25" ht="13.5">
       <c r="A32" s="5" t="s">
         <v>62</v>
       </c>
@@ -2087,7 +2300,7 @@
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
+      <c r="G32" s="8"/>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
@@ -2107,7 +2320,7 @@
       <c r="X32" s="5"/>
       <c r="Y32" s="5"/>
     </row>
-    <row r="33" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:25" ht="13.5">
       <c r="A33" s="5" t="s">
         <v>62</v>
       </c>
@@ -2122,8 +2335,12 @@
       </c>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
+      <c r="G33" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
@@ -2142,23 +2359,23 @@
       <c r="X33" s="5"/>
       <c r="Y33" s="5"/>
     </row>
-    <row r="34" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:25" ht="27">
       <c r="A34" s="5" t="s">
         <v>62</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>57</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="9"/>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
@@ -2177,15 +2394,15 @@
       <c r="X34" s="5"/>
       <c r="Y34" s="5"/>
     </row>
-    <row r="35" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:25" ht="27">
       <c r="A35" s="5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
@@ -2210,7 +2427,7 @@
       <c r="X35" s="5"/>
       <c r="Y35" s="5"/>
     </row>
-    <row r="36" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:25" ht="13.5">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -2237,23 +2454,23 @@
       <c r="X36" s="5"/>
       <c r="Y36" s="5"/>
     </row>
-    <row r="37" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:25" ht="33.6" customHeight="1">
       <c r="A37" s="5" t="s">
         <v>62</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D37" s="5"/>
-      <c r="E37" s="8" t="s">
-        <v>74</v>
+      <c r="E37" s="10" t="s">
+        <v>76</v>
       </c>
       <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="9"/>
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
@@ -2272,7 +2489,7 @@
       <c r="X37" s="5"/>
       <c r="Y37" s="5"/>
     </row>
-    <row r="38" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:25" ht="13.5">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -2299,23 +2516,27 @@
       <c r="X38" s="5"/>
       <c r="Y38" s="5"/>
     </row>
-    <row r="39" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:25" ht="13.5">
       <c r="A39" s="5" t="s">
         <v>54</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>57</v>
       </c>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
+      <c r="G39" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>113</v>
+      </c>
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
       <c r="K39" s="5"/>
@@ -2334,23 +2555,27 @@
       <c r="X39" s="5"/>
       <c r="Y39" s="5"/>
     </row>
-    <row r="40" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:25" ht="27">
       <c r="A40" s="5" t="s">
         <v>54</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>57</v>
       </c>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
+      <c r="G40" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
       <c r="K40" s="5"/>
@@ -2369,15 +2594,15 @@
       <c r="X40" s="5"/>
       <c r="Y40" s="5"/>
     </row>
-    <row r="41" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:25" ht="13.5">
       <c r="A41" s="5" t="s">
         <v>62</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
@@ -2402,7 +2627,7 @@
       <c r="X41" s="5"/>
       <c r="Y41" s="5"/>
     </row>
-    <row r="42" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:25" ht="13.5">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
@@ -2429,7 +2654,7 @@
       <c r="X42" s="5"/>
       <c r="Y42" s="5"/>
     </row>
-    <row r="43" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:25" ht="13.5">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -2456,7 +2681,7 @@
       <c r="X43" s="5"/>
       <c r="Y43" s="5"/>
     </row>
-    <row r="44" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:25" ht="13.5">
       <c r="A44" s="5" t="s">
         <v>34</v>
       </c>
@@ -2485,7 +2710,7 @@
       <c r="X44" s="5"/>
       <c r="Y44" s="5"/>
     </row>
-    <row r="45" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:25" ht="13.5">
       <c r="A45" s="4"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
@@ -2512,7 +2737,7 @@
       <c r="X45" s="5"/>
       <c r="Y45" s="5"/>
     </row>
-    <row r="46" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:25" ht="13.5">
       <c r="A46" s="4"/>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
@@ -2539,7 +2764,7 @@
       <c r="X46" s="5"/>
       <c r="Y46" s="5"/>
     </row>
-    <row r="47" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:25" ht="13.5">
       <c r="A47" s="4"/>
       <c r="B47" s="5"/>
       <c r="C47" s="7"/>
@@ -2566,7 +2791,7 @@
       <c r="X47" s="5"/>
       <c r="Y47" s="5"/>
     </row>
-    <row r="48" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:25" ht="13.5">
       <c r="A48" s="4"/>
       <c r="B48" s="5"/>
       <c r="C48" s="7"/>
@@ -2593,7 +2818,7 @@
       <c r="X48" s="5"/>
       <c r="Y48" s="5"/>
     </row>
-    <row r="49" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" spans="1:25" ht="13.5">
       <c r="A49" s="4"/>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
@@ -2620,9 +2845,9 @@
       <c r="X49" s="5"/>
       <c r="Y49" s="5"/>
     </row>
-    <row r="50" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" spans="1:25" ht="13.5">
       <c r="A50" s="4"/>
-      <c r="B50" s="9"/>
+      <c r="B50" s="11"/>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
@@ -2647,7 +2872,7 @@
       <c r="X50" s="4"/>
       <c r="Y50" s="4"/>
     </row>
-    <row r="51" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:25" ht="13.5">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -2674,7 +2899,7 @@
       <c r="X51" s="4"/>
       <c r="Y51" s="4"/>
     </row>
-    <row r="52" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" spans="1:25" ht="13.5">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -2701,7 +2926,7 @@
       <c r="X52" s="4"/>
       <c r="Y52" s="4"/>
     </row>
-    <row r="53" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" spans="1:25" ht="13.5">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
@@ -2728,7 +2953,7 @@
       <c r="X53" s="4"/>
       <c r="Y53" s="4"/>
     </row>
-    <row r="54" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:25" ht="13.5">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
@@ -2755,7 +2980,7 @@
       <c r="X54" s="4"/>
       <c r="Y54" s="4"/>
     </row>
-    <row r="55" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" spans="1:25" ht="13.5">
       <c r="A55" s="5"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
@@ -2782,7 +3007,7 @@
       <c r="X55" s="5"/>
       <c r="Y55" s="5"/>
     </row>
-    <row r="56" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" spans="1:25" ht="13.5">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="7"/>
@@ -2809,7 +3034,7 @@
       <c r="X56" s="4"/>
       <c r="Y56" s="4"/>
     </row>
-    <row r="57" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" spans="1:25" ht="13.5">
       <c r="A57" s="4"/>
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
@@ -2836,7 +3061,7 @@
       <c r="X57" s="5"/>
       <c r="Y57" s="5"/>
     </row>
-    <row r="58" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" spans="1:25" ht="13.5">
       <c r="A58" s="4"/>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
@@ -2863,7 +3088,7 @@
       <c r="X58" s="5"/>
       <c r="Y58" s="5"/>
     </row>
-    <row r="59" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" spans="1:25" ht="13.5">
       <c r="A59" s="5"/>
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
@@ -2890,7 +3115,7 @@
       <c r="X59" s="5"/>
       <c r="Y59" s="5"/>
     </row>
-    <row r="60" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" spans="1:25" ht="13.5">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
@@ -2917,7 +3142,7 @@
       <c r="X60" s="4"/>
       <c r="Y60" s="4"/>
     </row>
-    <row r="61" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" spans="1:25" ht="13.5">
       <c r="A61" s="4"/>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
@@ -2944,7 +3169,7 @@
       <c r="X61" s="5"/>
       <c r="Y61" s="5"/>
     </row>
-    <row r="62" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" spans="1:25" ht="13.5">
       <c r="A62" s="4"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
@@ -2971,7 +3196,7 @@
       <c r="X62" s="4"/>
       <c r="Y62" s="4"/>
     </row>
-    <row r="63" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" spans="1:25" ht="13.5">
       <c r="A63" s="5"/>
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
@@ -2998,446 +3223,423 @@
       <c r="X63" s="5"/>
       <c r="Y63" s="5"/>
     </row>
-    <row r="64" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="10"/>
+    <row r="64" spans="1:25" ht="13.5">
+      <c r="A64" s="12"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
-      <c r="G64" s="11"/>
-      <c r="H64" s="11"/>
-      <c r="I64" s="11"/>
-      <c r="J64" s="11"/>
-      <c r="K64" s="11"/>
-      <c r="L64" s="11"/>
-      <c r="M64" s="11"/>
-      <c r="N64" s="11"/>
-      <c r="O64" s="11"/>
-      <c r="P64" s="11"/>
-      <c r="Q64" s="11"/>
-      <c r="R64" s="11"/>
-      <c r="S64" s="11"/>
-      <c r="T64" s="11"/>
-      <c r="U64" s="11"/>
-      <c r="V64" s="11"/>
-      <c r="W64" s="11"/>
-      <c r="X64" s="11"/>
-      <c r="Y64" s="11"/>
-    </row>
-    <row r="65" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="10"/>
+      <c r="G64" s="13"/>
+      <c r="H64" s="13"/>
+      <c r="I64" s="13"/>
+      <c r="J64" s="13"/>
+      <c r="K64" s="13"/>
+      <c r="L64" s="13"/>
+      <c r="M64" s="13"/>
+      <c r="N64" s="13"/>
+      <c r="O64" s="13"/>
+      <c r="P64" s="13"/>
+      <c r="Q64" s="13"/>
+      <c r="R64" s="13"/>
+      <c r="S64" s="13"/>
+      <c r="T64" s="13"/>
+      <c r="U64" s="13"/>
+      <c r="V64" s="13"/>
+      <c r="W64" s="13"/>
+      <c r="X64" s="13"/>
+      <c r="Y64" s="13"/>
+    </row>
+    <row r="65" spans="1:25" ht="13.5">
+      <c r="A65" s="12"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
-      <c r="D65" s="11"/>
+      <c r="D65" s="13"/>
       <c r="E65" s="4"/>
       <c r="F65" s="4"/>
-      <c r="G65" s="11"/>
-      <c r="H65" s="11"/>
-      <c r="I65" s="11"/>
-      <c r="J65" s="11"/>
-      <c r="K65" s="11"/>
-      <c r="L65" s="11"/>
-      <c r="M65" s="11"/>
-      <c r="N65" s="11"/>
-      <c r="O65" s="11"/>
-      <c r="P65" s="11"/>
-      <c r="Q65" s="11"/>
-      <c r="R65" s="11"/>
-      <c r="S65" s="11"/>
-      <c r="T65" s="11"/>
-      <c r="U65" s="11"/>
-      <c r="V65" s="11"/>
-      <c r="W65" s="11"/>
-      <c r="X65" s="11"/>
-      <c r="Y65" s="11"/>
-    </row>
-    <row r="66" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="10"/>
+      <c r="G65" s="13"/>
+      <c r="H65" s="13"/>
+      <c r="I65" s="13"/>
+      <c r="J65" s="13"/>
+      <c r="K65" s="13"/>
+      <c r="L65" s="13"/>
+      <c r="M65" s="13"/>
+      <c r="N65" s="13"/>
+      <c r="O65" s="13"/>
+      <c r="P65" s="13"/>
+      <c r="Q65" s="13"/>
+      <c r="R65" s="13"/>
+      <c r="S65" s="13"/>
+      <c r="T65" s="13"/>
+      <c r="U65" s="13"/>
+      <c r="V65" s="13"/>
+      <c r="W65" s="13"/>
+      <c r="X65" s="13"/>
+      <c r="Y65" s="13"/>
+    </row>
+    <row r="66" spans="1:25" ht="13.5">
+      <c r="A66" s="12"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
-      <c r="D66" s="11"/>
+      <c r="D66" s="13"/>
       <c r="E66" s="4"/>
       <c r="F66" s="4"/>
-      <c r="G66" s="11"/>
-      <c r="H66" s="11"/>
-      <c r="I66" s="11"/>
-      <c r="J66" s="11"/>
-      <c r="K66" s="11"/>
-      <c r="L66" s="11"/>
-      <c r="M66" s="11"/>
-      <c r="N66" s="11"/>
-      <c r="O66" s="11"/>
-      <c r="P66" s="11"/>
-      <c r="Q66" s="11"/>
-      <c r="R66" s="11"/>
-      <c r="S66" s="11"/>
-      <c r="T66" s="11"/>
-      <c r="U66" s="11"/>
-      <c r="V66" s="11"/>
-      <c r="W66" s="11"/>
-      <c r="X66" s="11"/>
-      <c r="Y66" s="11"/>
+      <c r="G66" s="13"/>
+      <c r="H66" s="13"/>
+      <c r="I66" s="13"/>
+      <c r="J66" s="13"/>
+      <c r="K66" s="13"/>
+      <c r="L66" s="13"/>
+      <c r="M66" s="13"/>
+      <c r="N66" s="13"/>
+      <c r="O66" s="13"/>
+      <c r="P66" s="13"/>
+      <c r="Q66" s="13"/>
+      <c r="R66" s="13"/>
+      <c r="S66" s="13"/>
+      <c r="T66" s="13"/>
+      <c r="U66" s="13"/>
+      <c r="V66" s="13"/>
+      <c r="W66" s="13"/>
+      <c r="X66" s="13"/>
+      <c r="Y66" s="13"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1">
-    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+    <cfRule type="expression" dxfId="25" priority="2">
       <formula>AND(A1 = "type", COUNTIF($A$1:$A$1016, "begin group") = COUNTIF($A$1:$A$1016, "end group"))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="expression" dxfId="24" priority="3">
       <formula>OR(NOT(A1 = "type"), NOT(COUNTIF($A$1:$A$1007, "begin group") = COUNTIF($A$1:$A$1016, "end group")))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1">
-    <cfRule type="cellIs" priority="4" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="cellIs" dxfId="23" priority="4" operator="notEqual">
       <formula>"name"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1">
-    <cfRule type="notContainsText" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="label" dxfId="12"/>
+    <cfRule type="notContainsText" dxfId="22" priority="5" operator="notContains" text="label"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1">
-    <cfRule type="cellIs" priority="6" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
+    <cfRule type="cellIs" dxfId="21" priority="6" operator="notEqual">
       <formula>"required"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1">
-    <cfRule type="cellIs" priority="7" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
+    <cfRule type="cellIs" dxfId="20" priority="7" operator="notEqual">
       <formula>"relevant"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="cellIs" priority="8" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
+    <cfRule type="cellIs" dxfId="19" priority="8" operator="notEqual">
       <formula>"appearance"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1">
-    <cfRule type="cellIs" priority="9" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
+    <cfRule type="cellIs" dxfId="18" priority="9" operator="notEqual">
       <formula>"constraint"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="notContainsText" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="constraint_message" dxfId="17"/>
+    <cfRule type="notContainsText" dxfId="17" priority="10" operator="notContains" text="constraint_message"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1">
-    <cfRule type="cellIs" priority="11" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18">
+    <cfRule type="cellIs" dxfId="16" priority="11" operator="notEqual">
       <formula>"calculation"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1">
-    <cfRule type="cellIs" priority="12" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19">
+    <cfRule type="cellIs" dxfId="15" priority="12" operator="notEqual">
       <formula>"choice_filter"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1">
-    <cfRule type="notContainsText" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="hint" dxfId="20"/>
+    <cfRule type="notContainsText" dxfId="14" priority="13" operator="notContains" text="hint"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1">
-    <cfRule type="cellIs" priority="14" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="notEqual">
       <formula>"default"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:Y1">
-    <cfRule type="cellIs" priority="15" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22">
+    <cfRule type="cellIs" dxfId="12" priority="15" operator="notEqual">
       <formula>"media::image"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29:Y29">
-    <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26">
+    <cfRule type="expression" dxfId="11" priority="16">
       <formula>AND($A29="begin group", NOT($B29 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29:Y29">
-    <cfRule type="expression" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27">
+    <cfRule type="expression" dxfId="10" priority="17">
       <formula>AND($A29="end group", $B29 = "", $C29 = "", $D29 = "", $E29 = "", $F29 = "", $G29 = "", $H29 = "", $I29 = "", $J29 = "", $K29 = "", $L29 = "", $M29 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29:Y29">
-    <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
+    <cfRule type="expression" dxfId="9" priority="18">
       <formula>AND($A29="begin repeat", NOT($B29 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29:Y29">
-    <cfRule type="expression" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29">
+    <cfRule type="expression" dxfId="8" priority="19">
       <formula>AND($A29="end repeat", $B29 = "", $C29 = "", $D29 = "", $E29 = "", $F29 = "", $G29 = "", $H29 = "", $I29 = "", $J29 = "", $K29 = "", $L29 = "", $M29 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I29">
-    <cfRule type="expression" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30">
+    <cfRule type="expression" dxfId="7" priority="20">
       <formula>AND($I29 = "", $A29 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="expression" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31">
+    <cfRule type="expression" dxfId="6" priority="21">
       <formula>AND(AND(NOT($A29 = "end group"), NOT($A29 = "end repeat"), NOT($A29 = "")), $C29 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="expression" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32">
+    <cfRule type="expression" dxfId="5" priority="22">
       <formula>AND(AND(NOT($A29 = "end group"), NOT($A29 = "end repeat"), NOT($A29 = "")), $B29 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="expression" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33">
+    <cfRule type="expression" dxfId="4" priority="23">
       <formula>AND(NOT($G29 = ""), $H29 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="expression" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34">
+    <cfRule type="expression" dxfId="3" priority="24">
       <formula>COUNTIF($B$2:$B$1048,B29)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29:Y29">
-    <cfRule type="containsText" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="35"/>
+    <cfRule type="containsText" dxfId="2" priority="25" operator="containsText" text="calculate"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29:Y29">
-    <cfRule type="cellIs" priority="26" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="36">
+    <cfRule type="cellIs" dxfId="1" priority="26" operator="equal">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29">
-    <cfRule type="cellIs" priority="27" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="37">
+    <cfRule type="cellIs" dxfId="0" priority="27" operator="equal">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D2:D66" type="list">
+    <dataValidation type="list" allowBlank="1" sqref="D2:D66" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"yes,no"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:F65536"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.3571428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.2959183673469"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.8469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="15.3010204081633"/>
+    <col min="1" max="1" width="27.265625"/>
+    <col min="2" max="2" width="33.265625"/>
+    <col min="3" max="3" width="41.86328125"/>
+    <col min="4" max="1025" width="15.265625"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="B1" s="12" t="s">
+    <row r="1" spans="1:6" ht="13.9">
+      <c r="A1" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-    </row>
-    <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="C3" s="14" t="s">
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+    </row>
+    <row r="2" spans="1:6" ht="13.5">
+      <c r="A2" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="14" t="s">
+      <c r="B2" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="C2" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+    </row>
+    <row r="3" spans="1:6" ht="13.5">
+      <c r="A3" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="B6" s="14" t="s">
+      <c r="C3" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+    </row>
+    <row r="4" spans="1:6" ht="13.5">
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+    </row>
+    <row r="5" spans="1:6" ht="13.5">
+      <c r="A5" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-    </row>
-    <row r="7" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="B7" s="14" t="s">
+      <c r="B5" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C5" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-    </row>
-    <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="B8" s="14" t="s">
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+    </row>
+    <row r="6" spans="1:6" ht="13.5">
+      <c r="A6" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C6" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-    </row>
-    <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="B9" s="14" t="s">
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+    </row>
+    <row r="7" spans="1:6" ht="27">
+      <c r="A7" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C7" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-    </row>
-    <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+    </row>
+    <row r="8" spans="1:6" ht="13.5">
+      <c r="A8" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+    </row>
+    <row r="9" spans="1:6" ht="13.5">
+      <c r="A9" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+    </row>
+    <row r="1048576" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:F65536"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="15.3010204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="15.3010204081633"/>
+    <col min="1" max="2" width="15.265625"/>
+    <col min="3" max="3" width="24.59765625"/>
+    <col min="4" max="1025" width="15.265625"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="E1" s="12" t="s">
+    <row r="1" spans="1:6" ht="13.9">
+      <c r="A1" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="B1" s="14" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="14" t="s">
+      <c r="C1" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="D1" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="C2" s="15" t="n">
-        <f aca="true">NOW()</f>
-        <v>44060.4977124069</v>
-      </c>
-      <c r="D2" s="14" t="s">
+      <c r="E1" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="F1" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="F2" s="14"/>
-    </row>
-    <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    </row>
+    <row r="2" spans="1:6" ht="13.5">
+      <c r="A2" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="17">
+        <f ca="1">NOW()</f>
+        <v>44063.95655787037</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="F2" s="16"/>
+    </row>
+    <row r="1048576" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>